<commit_message>
RebuildExistingModel measure now works. Updated validate_sampling.rb to create buttons/dropdowns instead of using index.html for better browsing.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -5168,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ensure order of parameters from existing run is preserved for RebuildExistingModel measure. Fixes potential for measures being executed out of order.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -777,9 +777,6 @@
     <t>../seeds/EmptySeedModel.osm</t>
   </si>
   <si>
-    <t>../weather/national/*.*</t>
-  </si>
-  <si>
     <t>location_epw.txt</t>
   </si>
   <si>
@@ -1588,6 +1585,9 @@
   </si>
   <si>
     <t>../resources/</t>
+  </si>
+  <si>
+    <t>../weather/pnw/*.*</t>
   </si>
 </sst>
 </file>
@@ -5169,7 +5169,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5229,7 +5229,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
@@ -5340,7 +5340,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>77</v>
@@ -5362,7 +5362,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>156</v>
@@ -5675,7 +5675,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>247</v>
+        <v>517</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5731,13 +5731,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
+        <v>514</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="C44" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -5989,7 +5989,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>242</v>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -6063,7 +6063,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>235</v>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>238</v>
@@ -6112,7 +6112,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6139,7 +6139,7 @@
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>237</v>
@@ -6183,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>235</v>
@@ -6221,7 +6221,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>238</v>
@@ -6232,7 +6232,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6259,7 +6259,7 @@
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E11" s="41" t="s">
         <v>237</v>
@@ -6341,7 +6341,7 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>238</v>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="C14" s="41"/>
       <c r="D14" s="41" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>237</v>
@@ -6423,7 +6423,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>235</v>
@@ -6461,7 +6461,7 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>238</v>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>237</v>
@@ -6543,7 +6543,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>235</v>
@@ -6581,7 +6581,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>238</v>
@@ -6592,7 +6592,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6619,7 +6619,7 @@
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="41" t="s">
         <v>237</v>
@@ -6663,7 +6663,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>235</v>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>238</v>
@@ -6712,7 +6712,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>237</v>
@@ -6783,7 +6783,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>235</v>
@@ -6821,7 +6821,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>238</v>
@@ -6832,7 +6832,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -6859,7 +6859,7 @@
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E26" s="41" t="s">
         <v>237</v>
@@ -6903,7 +6903,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>235</v>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>238</v>
@@ -6952,7 +6952,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E29" s="41" t="s">
         <v>237</v>
@@ -7023,7 +7023,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>235</v>
@@ -7061,7 +7061,7 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>238</v>
@@ -7072,7 +7072,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E32" s="41" t="s">
         <v>237</v>
@@ -7143,7 +7143,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>235</v>
@@ -7181,7 +7181,7 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>238</v>
@@ -7192,7 +7192,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="41" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>237</v>
@@ -7263,7 +7263,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>235</v>
@@ -7301,7 +7301,7 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>238</v>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="C38" s="41"/>
       <c r="D38" s="41" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E38" s="41" t="s">
         <v>237</v>
@@ -7383,7 +7383,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>235</v>
@@ -7421,7 +7421,7 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>238</v>
@@ -7432,7 +7432,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7459,7 +7459,7 @@
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="41" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>237</v>
@@ -7503,7 +7503,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>235</v>
@@ -7541,7 +7541,7 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>238</v>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7579,7 +7579,7 @@
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="41" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E44" s="41" t="s">
         <v>237</v>
@@ -7623,7 +7623,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>235</v>
@@ -7661,7 +7661,7 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>238</v>
@@ -7672,7 +7672,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7699,7 +7699,7 @@
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E47" s="41" t="s">
         <v>237</v>
@@ -7743,7 +7743,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>235</v>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>238</v>
@@ -7792,7 +7792,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -7819,7 +7819,7 @@
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="41" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E50" s="41" t="s">
         <v>237</v>
@@ -7863,7 +7863,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>235</v>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>238</v>
@@ -7912,7 +7912,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -7939,7 +7939,7 @@
       </c>
       <c r="C53" s="41"/>
       <c r="D53" s="41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E53" s="41" t="s">
         <v>237</v>
@@ -7983,7 +7983,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>235</v>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>238</v>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="C56" s="41"/>
       <c r="D56" s="41" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E56" s="41" t="s">
         <v>237</v>
@@ -8103,7 +8103,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>235</v>
@@ -8141,7 +8141,7 @@
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>238</v>
@@ -8179,7 +8179,7 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E59" s="41" t="s">
         <v>237</v>
@@ -8223,7 +8223,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>235</v>
@@ -8261,7 +8261,7 @@
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>238</v>
@@ -8272,7 +8272,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8299,7 +8299,7 @@
       </c>
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>237</v>
@@ -8343,7 +8343,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C63" s="40" t="s">
         <v>235</v>
@@ -8381,7 +8381,7 @@
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>238</v>
@@ -8392,7 +8392,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="C65" s="41"/>
       <c r="D65" s="41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E65" s="41" t="s">
         <v>237</v>
@@ -8463,7 +8463,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>235</v>
@@ -8501,7 +8501,7 @@
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>238</v>
@@ -8512,7 +8512,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8539,7 +8539,7 @@
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>237</v>
@@ -8583,7 +8583,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C69" s="40" t="s">
         <v>235</v>
@@ -8621,7 +8621,7 @@
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>238</v>
@@ -8632,7 +8632,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8659,7 +8659,7 @@
       </c>
       <c r="C71" s="41"/>
       <c r="D71" s="41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E71" s="41" t="s">
         <v>237</v>
@@ -8703,7 +8703,7 @@
         <v>1</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C72" s="40" t="s">
         <v>235</v>
@@ -8741,7 +8741,7 @@
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>238</v>
@@ -8752,7 +8752,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -8779,7 +8779,7 @@
       </c>
       <c r="C74" s="41"/>
       <c r="D74" s="41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E74" s="41" t="s">
         <v>237</v>
@@ -8823,7 +8823,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C75" s="40" t="s">
         <v>235</v>
@@ -8861,7 +8861,7 @@
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>238</v>
@@ -8872,7 +8872,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8899,7 +8899,7 @@
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>237</v>
@@ -8943,7 +8943,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C78" s="40" t="s">
         <v>235</v>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>238</v>
@@ -8992,7 +8992,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -9019,7 +9019,7 @@
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>237</v>
@@ -9063,7 +9063,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C81" s="40" t="s">
         <v>235</v>
@@ -9101,7 +9101,7 @@
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>238</v>
@@ -9112,7 +9112,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9139,7 +9139,7 @@
       </c>
       <c r="C83" s="41"/>
       <c r="D83" s="41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E83" s="41" t="s">
         <v>237</v>
@@ -9183,7 +9183,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C84" s="40" t="s">
         <v>235</v>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>238</v>
@@ -9232,7 +9232,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9259,7 +9259,7 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>237</v>
@@ -9303,7 +9303,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C87" s="40" t="s">
         <v>235</v>
@@ -9341,7 +9341,7 @@
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>238</v>
@@ -9352,7 +9352,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9379,7 +9379,7 @@
       </c>
       <c r="C89" s="41"/>
       <c r="D89" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>237</v>
@@ -9423,7 +9423,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C90" s="40" t="s">
         <v>235</v>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>238</v>
@@ -9472,7 +9472,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="C92" s="41"/>
       <c r="D92" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E92" s="41" t="s">
         <v>237</v>
@@ -9543,7 +9543,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C93" s="40" t="s">
         <v>235</v>
@@ -9581,7 +9581,7 @@
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>238</v>
@@ -9592,7 +9592,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9619,7 +9619,7 @@
       </c>
       <c r="C95" s="41"/>
       <c r="D95" s="41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E95" s="41" t="s">
         <v>237</v>
@@ -9663,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>235</v>
@@ -9701,7 +9701,7 @@
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>238</v>
@@ -9712,7 +9712,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>237</v>
@@ -9783,7 +9783,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>235</v>
@@ -9821,7 +9821,7 @@
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>238</v>
@@ -9832,7 +9832,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9859,7 +9859,7 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>237</v>
@@ -9903,7 +9903,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>235</v>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="C103" s="10"/>
       <c r="D103" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>238</v>
@@ -9952,7 +9952,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -9979,7 +9979,7 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>237</v>
@@ -10023,7 +10023,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>235</v>
@@ -10061,7 +10061,7 @@
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E106" s="10" t="s">
         <v>238</v>
@@ -10072,7 +10072,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10099,7 +10099,7 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>237</v>
@@ -10143,7 +10143,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C108" s="40" t="s">
         <v>235</v>
@@ -10181,7 +10181,7 @@
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E109" s="10" t="s">
         <v>238</v>
@@ -10192,7 +10192,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10219,7 +10219,7 @@
       </c>
       <c r="C110" s="41"/>
       <c r="D110" s="41" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E110" s="41" t="s">
         <v>237</v>
@@ -10263,7 +10263,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C111" s="40" t="s">
         <v>235</v>
@@ -10301,7 +10301,7 @@
       </c>
       <c r="C112" s="10"/>
       <c r="D112" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E112" s="10" t="s">
         <v>238</v>
@@ -10312,7 +10312,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10339,7 +10339,7 @@
       </c>
       <c r="C113" s="41"/>
       <c r="D113" s="41" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E113" s="41" t="s">
         <v>237</v>
@@ -10383,7 +10383,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C114" s="40" t="s">
         <v>235</v>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>238</v>
@@ -10432,7 +10432,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10459,7 +10459,7 @@
       </c>
       <c r="C116" s="41"/>
       <c r="D116" s="41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>237</v>
@@ -10503,7 +10503,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="C118" s="10"/>
       <c r="D118" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E118" s="10" t="s">
         <v>238</v>
@@ -10552,7 +10552,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10579,7 +10579,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10623,7 +10623,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10661,7 +10661,7 @@
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>238</v>
@@ -10672,7 +10672,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10699,7 +10699,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10743,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -10781,7 +10781,7 @@
       </c>
       <c r="C124" s="10"/>
       <c r="D124" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E124" s="10" t="s">
         <v>238</v>
@@ -10792,7 +10792,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10819,7 +10819,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -10863,7 +10863,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -10901,7 +10901,7 @@
       </c>
       <c r="C127" s="10"/>
       <c r="D127" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E127" s="10" t="s">
         <v>238</v>
@@ -10912,7 +10912,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10939,7 +10939,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -10983,7 +10983,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11021,7 +11021,7 @@
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>238</v>
@@ -11032,7 +11032,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11059,7 +11059,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11103,7 +11103,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11141,7 +11141,7 @@
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>238</v>
@@ -11152,7 +11152,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11179,7 +11179,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11223,7 +11223,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11261,7 +11261,7 @@
       </c>
       <c r="C136" s="10"/>
       <c r="D136" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E136" s="10" t="s">
         <v>238</v>
@@ -11272,7 +11272,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11299,7 +11299,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11343,7 +11343,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11381,7 +11381,7 @@
       </c>
       <c r="C139" s="10"/>
       <c r="D139" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>238</v>
@@ -11392,7 +11392,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11419,7 +11419,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11463,7 +11463,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11501,7 +11501,7 @@
       </c>
       <c r="C142" s="10"/>
       <c r="D142" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E142" s="10" t="s">
         <v>238</v>
@@ -11512,7 +11512,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11539,7 +11539,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11583,7 +11583,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11621,7 +11621,7 @@
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E145" s="10" t="s">
         <v>238</v>
@@ -11632,7 +11632,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11659,7 +11659,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -11703,7 +11703,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -11741,7 +11741,7 @@
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E148" s="10" t="s">
         <v>238</v>
@@ -11752,7 +11752,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11779,7 +11779,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -11823,7 +11823,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -11861,7 +11861,7 @@
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E151" s="10" t="s">
         <v>238</v>
@@ -11872,7 +11872,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11899,7 +11899,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -11943,7 +11943,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E154" s="10" t="s">
         <v>238</v>
@@ -11992,7 +11992,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12019,7 +12019,7 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12063,7 +12063,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12101,7 +12101,7 @@
       </c>
       <c r="C157" s="10"/>
       <c r="D157" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E157" s="10" t="s">
         <v>238</v>
@@ -12112,7 +12112,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12139,7 +12139,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12183,7 +12183,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12221,7 +12221,7 @@
       </c>
       <c r="C160" s="10"/>
       <c r="D160" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>238</v>
@@ -12232,7 +12232,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12259,7 +12259,7 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12303,16 +12303,16 @@
         <v>1</v>
       </c>
       <c r="B162" s="42" t="s">
+        <v>327</v>
+      </c>
+      <c r="C162" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="C162" s="42" t="s">
-        <v>329</v>
-      </c>
       <c r="D162" s="42" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E162" s="42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F162" s="42"/>
       <c r="G162" s="42"/>
@@ -12339,16 +12339,16 @@
         <v>1</v>
       </c>
       <c r="B163" s="42" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C163" s="42" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D163" s="42" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E163" s="42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -12507,16 +12507,16 @@
     </row>
     <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
@@ -12534,16 +12534,16 @@
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G5" s="15" t="b">
         <v>0</v>
@@ -12561,16 +12561,16 @@
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G6" s="15" t="b">
         <v>0</v>
@@ -12588,16 +12588,16 @@
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G7" s="15" t="b">
         <v>0</v>
@@ -12615,16 +12615,16 @@
     </row>
     <row r="8" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G8" s="15" t="b">
         <v>0</v>
@@ -12642,16 +12642,16 @@
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G9" s="15" t="b">
         <v>0</v>
@@ -12669,16 +12669,16 @@
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G10" s="15" t="b">
         <v>0</v>
@@ -12696,16 +12696,16 @@
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G11" s="15" t="b">
         <v>0</v>
@@ -12723,16 +12723,16 @@
     </row>
     <row r="12" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G12" s="15" t="b">
         <v>0</v>
@@ -12750,16 +12750,16 @@
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G13" s="15" t="b">
         <v>0</v>
@@ -12777,16 +12777,16 @@
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -12804,16 +12804,16 @@
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G15" s="15" t="b">
         <v>0</v>
@@ -12831,16 +12831,16 @@
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -12858,14 +12858,14 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B17" s="21"/>
       <c r="D17" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -12879,14 +12879,14 @@
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B18" s="21"/>
       <c r="D18" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -12900,16 +12900,16 @@
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -12927,16 +12927,16 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -12954,16 +12954,16 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>0</v>
@@ -12981,16 +12981,16 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>0</v>
@@ -13008,16 +13008,16 @@
     </row>
     <row r="23" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>0</v>
@@ -13035,14 +13035,14 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B24" s="21"/>
       <c r="D24" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>0</v>
@@ -13056,14 +13056,14 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B25" s="21"/>
       <c r="D25" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G25" s="15" t="b">
         <v>0</v>
@@ -13077,14 +13077,14 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G26" s="15" t="b">
         <v>0</v>
@@ -13098,14 +13098,14 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G27" s="15" t="b">
         <v>0</v>
@@ -13119,14 +13119,14 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B28" s="21"/>
       <c r="D28" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G28" s="15" t="b">
         <v>0</v>
@@ -13140,14 +13140,14 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B29" s="21"/>
       <c r="D29" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G29" s="15" t="b">
         <v>0</v>
@@ -13161,14 +13161,14 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B30" s="21"/>
       <c r="D30" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G30" s="15" t="b">
         <v>0</v>
@@ -13182,14 +13182,14 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B31" s="21"/>
       <c r="D31" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G31" s="15" t="b">
         <v>0</v>
@@ -13203,14 +13203,14 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="44" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B32" s="21"/>
       <c r="D32" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G32" s="15" t="b">
         <v>0</v>
@@ -13224,14 +13224,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="44" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B33" s="21"/>
       <c r="D33" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G33" s="15" t="b">
         <v>0</v>
@@ -13245,14 +13245,14 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G34" s="15" t="b">
         <v>0</v>
@@ -13266,14 +13266,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G35" s="15" t="b">
         <v>0</v>
@@ -13287,14 +13287,14 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B36" s="21"/>
       <c r="D36" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G36" s="15" t="b">
         <v>0</v>
@@ -13308,14 +13308,14 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B37" s="21"/>
       <c r="D37" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G37" s="15" t="b">
         <v>0</v>
@@ -13329,14 +13329,14 @@
     </row>
     <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B38" s="21"/>
       <c r="D38" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G38" s="15" t="b">
         <v>0</v>
@@ -13350,14 +13350,14 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B39" s="21"/>
       <c r="D39" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G39" s="15" t="b">
         <v>0</v>
@@ -13371,14 +13371,14 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G40" s="15" t="b">
         <v>0</v>
@@ -13392,14 +13392,14 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G41" s="15" t="b">
         <v>0</v>
@@ -13413,14 +13413,14 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G42" s="15" t="b">
         <v>0</v>
@@ -13434,14 +13434,14 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G43" s="15" t="b">
         <v>0</v>
@@ -13455,14 +13455,14 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G44" s="15" t="b">
         <v>0</v>
@@ -13476,14 +13476,14 @@
     </row>
     <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G45" s="15" t="b">
         <v>0</v>
@@ -13497,14 +13497,14 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G46" s="15" t="b">
         <v>0</v>
@@ -13518,15 +13518,15 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G47" s="15" t="b">
         <v>0</v>
@@ -13540,15 +13540,15 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G48" s="15" t="b">
         <v>0</v>
@@ -13562,15 +13562,15 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G49" s="15" t="b">
         <v>0</v>
@@ -13584,15 +13584,15 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E50" s="22"/>
       <c r="F50" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G50" s="15" t="b">
         <v>0</v>
@@ -13606,15 +13606,15 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G51" s="15" t="b">
         <v>0</v>
@@ -13628,15 +13628,15 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B52" s="21"/>
       <c r="D52" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G52" s="15" t="b">
         <v>0</v>
@@ -13650,15 +13650,15 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G53" s="15" t="b">
         <v>0</v>
@@ -13672,15 +13672,15 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G54" s="15" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Add foundation type as dependency for foundation insulation distributions.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -5168,8 +5168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added HVAC measures and probability distributions into the workflow. Addresses #1.
TODO:
Probabilities are merely placeholders at the moment.
Need to update OS version to fix 1-spd ASHP errors.
Need to update approach for setpoints once https://github.com/NREL/OpenStudio-Beopt/issues/19 is implemented.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="543">
   <si>
     <t>type</t>
   </si>
@@ -1588,6 +1588,81 @@
   </si>
   <si>
     <t>../weather/pnw/*.*</t>
+  </si>
+  <si>
+    <t>hvac_system_combined.txt</t>
+  </si>
+  <si>
+    <t>Set HVAC System Combined</t>
+  </si>
+  <si>
+    <t>HVAC System Combined Sample Value</t>
+  </si>
+  <si>
+    <t>Set HVAC System Is Combined</t>
+  </si>
+  <si>
+    <t>HVAC System Is Combined Sample Value</t>
+  </si>
+  <si>
+    <t>hvac_system_is_combined.txt</t>
+  </si>
+  <si>
+    <t>HVAC System Is Combined</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.hvac_system_is_combined</t>
+  </si>
+  <si>
+    <t>HVAC System Combined</t>
+  </si>
+  <si>
+    <t>HVAC System Cooling</t>
+  </si>
+  <si>
+    <t>HVAC System Heating</t>
+  </si>
+  <si>
+    <t>Set HVAC System Heating</t>
+  </si>
+  <si>
+    <t>Set HVAC System Cooling</t>
+  </si>
+  <si>
+    <t>HVAC System Cooling Sample Value</t>
+  </si>
+  <si>
+    <t>HVAC System Heating Sample Value</t>
+  </si>
+  <si>
+    <t>hvac_system_heating.txt</t>
+  </si>
+  <si>
+    <t>hvac_system_cooling.txt</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.hvac_system_cooling</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.hvac_system_heating</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.hvac_system_combined</t>
+  </si>
+  <si>
+    <t>Set HVAC Setpoints</t>
+  </si>
+  <si>
+    <t>HVAC Setpoints Sample Value</t>
+  </si>
+  <si>
+    <t>hvac_setpoints.txt</t>
+  </si>
+  <si>
+    <t>HVAC Setpoints</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.hvac_setpoints</t>
   </si>
 </sst>
 </file>
@@ -5168,7 +5243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -5805,9 +5880,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z163"/>
+  <dimension ref="A1:Z178"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10503,7 +10580,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>330</v>
+        <v>538</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10552,7 +10629,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>332</v>
+        <v>540</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10579,7 +10656,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>331</v>
+        <v>539</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10623,7 +10700,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>336</v>
+        <v>521</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10672,7 +10749,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>338</v>
+        <v>523</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10699,7 +10776,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>337</v>
+        <v>522</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10743,7 +10820,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>342</v>
+        <v>519</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -10792,7 +10869,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>344</v>
+        <v>518</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10819,7 +10896,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>343</v>
+        <v>520</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -10863,7 +10940,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>345</v>
+        <v>529</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -10912,7 +10989,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>347</v>
+        <v>533</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -10939,7 +11016,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>346</v>
+        <v>532</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -10983,7 +11060,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>348</v>
+        <v>530</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11032,7 +11109,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>350</v>
+        <v>534</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11059,7 +11136,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>349</v>
+        <v>531</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11103,7 +11180,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>503</v>
+        <v>330</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11152,7 +11229,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>505</v>
+        <v>332</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11179,7 +11256,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>504</v>
+        <v>331</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11223,7 +11300,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11272,7 +11349,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11299,7 +11376,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11343,7 +11420,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>449</v>
+        <v>342</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11392,7 +11469,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>454</v>
+        <v>344</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11419,7 +11496,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>450</v>
+        <v>343</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11463,7 +11540,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>464</v>
+        <v>345</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11512,7 +11589,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>466</v>
+        <v>347</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11539,7 +11616,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>465</v>
+        <v>346</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11583,7 +11660,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>467</v>
+        <v>348</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11632,7 +11709,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>469</v>
+        <v>350</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11659,7 +11736,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>468</v>
+        <v>349</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -11703,7 +11780,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>451</v>
+        <v>503</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -11752,7 +11829,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>453</v>
+        <v>505</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11779,7 +11856,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>452</v>
+        <v>504</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -11823,7 +11900,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>455</v>
+        <v>351</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -11872,7 +11949,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>457</v>
+        <v>353</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11899,7 +11976,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>456</v>
+        <v>352</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -11943,7 +12020,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>477</v>
+        <v>449</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -11992,7 +12069,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12019,7 +12096,7 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>478</v>
+        <v>450</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12063,7 +12140,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12112,7 +12189,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12139,7 +12216,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12183,7 +12260,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12232,7 +12309,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12252,14 +12329,14 @@
       <c r="Y160" s="15"/>
       <c r="Z160" s="15"/>
     </row>
-    <row r="161" spans="1:24" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="41"/>
       <c r="B161" s="41" t="s">
         <v>21</v>
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12298,77 +12375,677 @@
       <c r="W161" s="41"/>
       <c r="X161" s="41"/>
     </row>
-    <row r="162" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="42" t="b">
+    <row r="162" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B162" s="42" t="s">
+      <c r="B162" s="40" t="s">
+        <v>451</v>
+      </c>
+      <c r="C162" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D162" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E162" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F162" s="40"/>
+      <c r="G162" s="40"/>
+      <c r="H162" s="40"/>
+      <c r="I162" s="40"/>
+      <c r="J162" s="40"/>
+      <c r="K162" s="40"/>
+      <c r="L162" s="40"/>
+      <c r="M162" s="40"/>
+      <c r="N162" s="40"/>
+      <c r="O162" s="40"/>
+      <c r="P162" s="40"/>
+      <c r="Q162" s="40"/>
+      <c r="R162" s="40"/>
+      <c r="S162" s="40"/>
+      <c r="T162" s="40"/>
+      <c r="U162" s="40"/>
+      <c r="V162" s="40"/>
+      <c r="W162" s="40"/>
+      <c r="X162" s="40"/>
+    </row>
+    <row r="163" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="10"/>
+      <c r="B163" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E163" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F163" s="10"/>
+      <c r="G163" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H163" s="10"/>
+      <c r="I163" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="J163" s="10"/>
+      <c r="K163" s="10"/>
+      <c r="L163" s="10"/>
+      <c r="M163" s="10"/>
+      <c r="N163" s="10"/>
+      <c r="O163" s="10"/>
+      <c r="P163" s="10"/>
+      <c r="Q163" s="10"/>
+      <c r="R163" s="10"/>
+      <c r="S163" s="10"/>
+      <c r="T163" s="10"/>
+      <c r="U163" s="10"/>
+      <c r="V163" s="10"/>
+      <c r="W163" s="10"/>
+      <c r="X163" s="10"/>
+      <c r="Y163" s="15"/>
+      <c r="Z163" s="15"/>
+    </row>
+    <row r="164" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A164" s="41"/>
+      <c r="B164" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C164" s="41"/>
+      <c r="D164" s="41" t="s">
+        <v>452</v>
+      </c>
+      <c r="E164" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F164" s="41"/>
+      <c r="G164" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H164" s="41"/>
+      <c r="I164" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J164" s="41"/>
+      <c r="K164" s="41">
+        <v>0</v>
+      </c>
+      <c r="L164" s="41">
+        <v>1</v>
+      </c>
+      <c r="M164" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N164" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O164" s="41"/>
+      <c r="P164" s="41"/>
+      <c r="Q164" s="41"/>
+      <c r="R164" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S164" s="41"/>
+      <c r="T164" s="41"/>
+      <c r="U164" s="41"/>
+      <c r="V164" s="41"/>
+      <c r="W164" s="41"/>
+      <c r="X164" s="41"/>
+    </row>
+    <row r="165" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A165" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B165" s="40" t="s">
+        <v>455</v>
+      </c>
+      <c r="C165" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D165" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E165" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F165" s="40"/>
+      <c r="G165" s="40"/>
+      <c r="H165" s="40"/>
+      <c r="I165" s="40"/>
+      <c r="J165" s="40"/>
+      <c r="K165" s="40"/>
+      <c r="L165" s="40"/>
+      <c r="M165" s="40"/>
+      <c r="N165" s="40"/>
+      <c r="O165" s="40"/>
+      <c r="P165" s="40"/>
+      <c r="Q165" s="40"/>
+      <c r="R165" s="40"/>
+      <c r="S165" s="40"/>
+      <c r="T165" s="40"/>
+      <c r="U165" s="40"/>
+      <c r="V165" s="40"/>
+      <c r="W165" s="40"/>
+      <c r="X165" s="40"/>
+    </row>
+    <row r="166" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="10"/>
+      <c r="B166" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C166" s="10"/>
+      <c r="D166" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E166" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F166" s="10"/>
+      <c r="G166" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H166" s="10"/>
+      <c r="I166" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="J166" s="10"/>
+      <c r="K166" s="10"/>
+      <c r="L166" s="10"/>
+      <c r="M166" s="10"/>
+      <c r="N166" s="10"/>
+      <c r="O166" s="10"/>
+      <c r="P166" s="10"/>
+      <c r="Q166" s="10"/>
+      <c r="R166" s="10"/>
+      <c r="S166" s="10"/>
+      <c r="T166" s="10"/>
+      <c r="U166" s="10"/>
+      <c r="V166" s="10"/>
+      <c r="W166" s="10"/>
+      <c r="X166" s="10"/>
+      <c r="Y166" s="15"/>
+      <c r="Z166" s="15"/>
+    </row>
+    <row r="167" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A167" s="41"/>
+      <c r="B167" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C167" s="41"/>
+      <c r="D167" s="41" t="s">
+        <v>456</v>
+      </c>
+      <c r="E167" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F167" s="41"/>
+      <c r="G167" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H167" s="41"/>
+      <c r="I167" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J167" s="41"/>
+      <c r="K167" s="41">
+        <v>0</v>
+      </c>
+      <c r="L167" s="41">
+        <v>1</v>
+      </c>
+      <c r="M167" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N167" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O167" s="41"/>
+      <c r="P167" s="41"/>
+      <c r="Q167" s="41"/>
+      <c r="R167" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S167" s="41"/>
+      <c r="T167" s="41"/>
+      <c r="U167" s="41"/>
+      <c r="V167" s="41"/>
+      <c r="W167" s="41"/>
+      <c r="X167" s="41"/>
+    </row>
+    <row r="168" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A168" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B168" s="40" t="s">
+        <v>477</v>
+      </c>
+      <c r="C168" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D168" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E168" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F168" s="40"/>
+      <c r="G168" s="40"/>
+      <c r="H168" s="40"/>
+      <c r="I168" s="40"/>
+      <c r="J168" s="40"/>
+      <c r="K168" s="40"/>
+      <c r="L168" s="40"/>
+      <c r="M168" s="40"/>
+      <c r="N168" s="40"/>
+      <c r="O168" s="40"/>
+      <c r="P168" s="40"/>
+      <c r="Q168" s="40"/>
+      <c r="R168" s="40"/>
+      <c r="S168" s="40"/>
+      <c r="T168" s="40"/>
+      <c r="U168" s="40"/>
+      <c r="V168" s="40"/>
+      <c r="W168" s="40"/>
+      <c r="X168" s="40"/>
+    </row>
+    <row r="169" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="10"/>
+      <c r="B169" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E169" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F169" s="10"/>
+      <c r="G169" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H169" s="10"/>
+      <c r="I169" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="J169" s="10"/>
+      <c r="K169" s="10"/>
+      <c r="L169" s="10"/>
+      <c r="M169" s="10"/>
+      <c r="N169" s="10"/>
+      <c r="O169" s="10"/>
+      <c r="P169" s="10"/>
+      <c r="Q169" s="10"/>
+      <c r="R169" s="10"/>
+      <c r="S169" s="10"/>
+      <c r="T169" s="10"/>
+      <c r="U169" s="10"/>
+      <c r="V169" s="10"/>
+      <c r="W169" s="10"/>
+      <c r="X169" s="10"/>
+      <c r="Y169" s="15"/>
+      <c r="Z169" s="15"/>
+    </row>
+    <row r="170" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A170" s="41"/>
+      <c r="B170" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C170" s="41"/>
+      <c r="D170" s="41" t="s">
+        <v>478</v>
+      </c>
+      <c r="E170" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F170" s="41"/>
+      <c r="G170" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H170" s="41"/>
+      <c r="I170" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J170" s="41"/>
+      <c r="K170" s="41">
+        <v>0</v>
+      </c>
+      <c r="L170" s="41">
+        <v>1</v>
+      </c>
+      <c r="M170" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N170" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O170" s="41"/>
+      <c r="P170" s="41"/>
+      <c r="Q170" s="41"/>
+      <c r="R170" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S170" s="41"/>
+      <c r="T170" s="41"/>
+      <c r="U170" s="41"/>
+      <c r="V170" s="41"/>
+      <c r="W170" s="41"/>
+      <c r="X170" s="41"/>
+    </row>
+    <row r="171" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B171" s="40" t="s">
+        <v>458</v>
+      </c>
+      <c r="C171" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D171" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E171" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F171" s="40"/>
+      <c r="G171" s="40"/>
+      <c r="H171" s="40"/>
+      <c r="I171" s="40"/>
+      <c r="J171" s="40"/>
+      <c r="K171" s="40"/>
+      <c r="L171" s="40"/>
+      <c r="M171" s="40"/>
+      <c r="N171" s="40"/>
+      <c r="O171" s="40"/>
+      <c r="P171" s="40"/>
+      <c r="Q171" s="40"/>
+      <c r="R171" s="40"/>
+      <c r="S171" s="40"/>
+      <c r="T171" s="40"/>
+      <c r="U171" s="40"/>
+      <c r="V171" s="40"/>
+      <c r="W171" s="40"/>
+      <c r="X171" s="40"/>
+    </row>
+    <row r="172" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="10"/>
+      <c r="B172" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E172" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F172" s="10"/>
+      <c r="G172" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H172" s="10"/>
+      <c r="I172" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="J172" s="10"/>
+      <c r="K172" s="10"/>
+      <c r="L172" s="10"/>
+      <c r="M172" s="10"/>
+      <c r="N172" s="10"/>
+      <c r="O172" s="10"/>
+      <c r="P172" s="10"/>
+      <c r="Q172" s="10"/>
+      <c r="R172" s="10"/>
+      <c r="S172" s="10"/>
+      <c r="T172" s="10"/>
+      <c r="U172" s="10"/>
+      <c r="V172" s="10"/>
+      <c r="W172" s="10"/>
+      <c r="X172" s="10"/>
+      <c r="Y172" s="15"/>
+      <c r="Z172" s="15"/>
+    </row>
+    <row r="173" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A173" s="41"/>
+      <c r="B173" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C173" s="41"/>
+      <c r="D173" s="41" t="s">
+        <v>459</v>
+      </c>
+      <c r="E173" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F173" s="41"/>
+      <c r="G173" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H173" s="41"/>
+      <c r="I173" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J173" s="41"/>
+      <c r="K173" s="41">
+        <v>0</v>
+      </c>
+      <c r="L173" s="41">
+        <v>1</v>
+      </c>
+      <c r="M173" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N173" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O173" s="41"/>
+      <c r="P173" s="41"/>
+      <c r="Q173" s="41"/>
+      <c r="R173" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S173" s="41"/>
+      <c r="T173" s="41"/>
+      <c r="U173" s="41"/>
+      <c r="V173" s="41"/>
+      <c r="W173" s="41"/>
+      <c r="X173" s="41"/>
+    </row>
+    <row r="174" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A174" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B174" s="40" t="s">
+        <v>461</v>
+      </c>
+      <c r="C174" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D174" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E174" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F174" s="40"/>
+      <c r="G174" s="40"/>
+      <c r="H174" s="40"/>
+      <c r="I174" s="40"/>
+      <c r="J174" s="40"/>
+      <c r="K174" s="40"/>
+      <c r="L174" s="40"/>
+      <c r="M174" s="40"/>
+      <c r="N174" s="40"/>
+      <c r="O174" s="40"/>
+      <c r="P174" s="40"/>
+      <c r="Q174" s="40"/>
+      <c r="R174" s="40"/>
+      <c r="S174" s="40"/>
+      <c r="T174" s="40"/>
+      <c r="U174" s="40"/>
+      <c r="V174" s="40"/>
+      <c r="W174" s="40"/>
+      <c r="X174" s="40"/>
+    </row>
+    <row r="175" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="10"/>
+      <c r="B175" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C175" s="10"/>
+      <c r="D175" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E175" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F175" s="10"/>
+      <c r="G175" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H175" s="10"/>
+      <c r="I175" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="J175" s="10"/>
+      <c r="K175" s="10"/>
+      <c r="L175" s="10"/>
+      <c r="M175" s="10"/>
+      <c r="N175" s="10"/>
+      <c r="O175" s="10"/>
+      <c r="P175" s="10"/>
+      <c r="Q175" s="10"/>
+      <c r="R175" s="10"/>
+      <c r="S175" s="10"/>
+      <c r="T175" s="10"/>
+      <c r="U175" s="10"/>
+      <c r="V175" s="10"/>
+      <c r="W175" s="10"/>
+      <c r="X175" s="10"/>
+      <c r="Y175" s="15"/>
+      <c r="Z175" s="15"/>
+    </row>
+    <row r="176" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A176" s="41"/>
+      <c r="B176" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C176" s="41"/>
+      <c r="D176" s="41" t="s">
+        <v>462</v>
+      </c>
+      <c r="E176" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F176" s="41"/>
+      <c r="G176" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H176" s="41"/>
+      <c r="I176" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J176" s="41"/>
+      <c r="K176" s="41">
+        <v>0</v>
+      </c>
+      <c r="L176" s="41">
+        <v>1</v>
+      </c>
+      <c r="M176" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N176" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O176" s="41"/>
+      <c r="P176" s="41"/>
+      <c r="Q176" s="41"/>
+      <c r="R176" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S176" s="41"/>
+      <c r="T176" s="41"/>
+      <c r="U176" s="41"/>
+      <c r="V176" s="41"/>
+      <c r="W176" s="41"/>
+      <c r="X176" s="41"/>
+    </row>
+    <row r="177" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A177" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B177" s="42" t="s">
         <v>327</v>
       </c>
-      <c r="C162" s="42" t="s">
+      <c r="C177" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="D162" s="42" t="s">
+      <c r="D177" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="E162" s="42" t="s">
+      <c r="E177" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="F162" s="42"/>
-      <c r="G162" s="42"/>
-      <c r="H162" s="43"/>
-      <c r="I162" s="43"/>
-      <c r="J162" s="42"/>
-      <c r="K162" s="42"/>
-      <c r="L162" s="42"/>
-      <c r="M162" s="42"/>
-      <c r="N162" s="42"/>
-      <c r="O162" s="42"/>
-      <c r="P162" s="42"/>
-      <c r="Q162" s="42"/>
-      <c r="R162" s="42"/>
-      <c r="S162" s="42"/>
-      <c r="T162" s="42"/>
-      <c r="U162" s="42"/>
-      <c r="V162" s="42"/>
-      <c r="W162" s="42"/>
-      <c r="X162" s="42"/>
-    </row>
-    <row r="163" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="42" t="b">
+      <c r="F177" s="42"/>
+      <c r="G177" s="42"/>
+      <c r="H177" s="43"/>
+      <c r="I177" s="43"/>
+      <c r="J177" s="42"/>
+      <c r="K177" s="42"/>
+      <c r="L177" s="42"/>
+      <c r="M177" s="42"/>
+      <c r="N177" s="42"/>
+      <c r="O177" s="42"/>
+      <c r="P177" s="42"/>
+      <c r="Q177" s="42"/>
+      <c r="R177" s="42"/>
+      <c r="S177" s="42"/>
+      <c r="T177" s="42"/>
+      <c r="U177" s="42"/>
+      <c r="V177" s="42"/>
+      <c r="W177" s="42"/>
+      <c r="X177" s="42"/>
+    </row>
+    <row r="178" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A178" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B163" s="42" t="s">
+      <c r="B178" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C163" s="42" t="s">
+      <c r="C178" s="42" t="s">
         <v>512</v>
       </c>
-      <c r="D163" s="42" t="s">
+      <c r="D178" s="42" t="s">
         <v>512</v>
       </c>
-      <c r="E163" s="42" t="s">
+      <c r="E178" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="F163" s="42"/>
-      <c r="G163" s="42"/>
-      <c r="H163" s="43"/>
-      <c r="I163" s="43"/>
-      <c r="J163" s="42"/>
-      <c r="K163" s="42"/>
-      <c r="L163" s="42"/>
-      <c r="M163" s="42"/>
-      <c r="N163" s="42"/>
-      <c r="O163" s="42"/>
-      <c r="P163" s="42"/>
-      <c r="Q163" s="42"/>
-      <c r="R163" s="42"/>
-      <c r="S163" s="42"/>
-      <c r="T163" s="42"/>
-      <c r="U163" s="42"/>
-      <c r="V163" s="42"/>
-      <c r="W163" s="42"/>
-      <c r="X163" s="42"/>
+      <c r="F178" s="42"/>
+      <c r="G178" s="42"/>
+      <c r="H178" s="43"/>
+      <c r="I178" s="43"/>
+      <c r="J178" s="42"/>
+      <c r="K178" s="42"/>
+      <c r="L178" s="42"/>
+      <c r="M178" s="42"/>
+      <c r="N178" s="42"/>
+      <c r="O178" s="42"/>
+      <c r="P178" s="42"/>
+      <c r="Q178" s="42"/>
+      <c r="R178" s="42"/>
+      <c r="S178" s="42"/>
+      <c r="T178" s="42"/>
+      <c r="U178" s="42"/>
+      <c r="V178" s="42"/>
+      <c r="W178" s="42"/>
+      <c r="X178" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -12387,11 +13064,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13369,13 +14046,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="s">
-        <v>390</v>
+        <v>541</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>397</v>
+        <v>542</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>329</v>
@@ -13390,13 +14067,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="s">
-        <v>391</v>
+        <v>524</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>425</v>
+        <v>525</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>329</v>
@@ -13411,13 +14088,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
-        <v>392</v>
+        <v>526</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>398</v>
+        <v>537</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>329</v>
@@ -13432,13 +14109,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
-        <v>393</v>
+        <v>528</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>426</v>
+        <v>536</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>329</v>
@@ -13453,13 +14130,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>394</v>
+        <v>527</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>427</v>
+        <v>535</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>329</v>
@@ -13474,13 +14151,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>506</v>
+        <v>390</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>507</v>
+        <v>397</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>329</v>
@@ -13497,11 +14174,11 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>329</v>
@@ -13518,13 +14195,12 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>470</v>
+        <v>392</v>
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="E47" s="22"/>
+        <v>398</v>
+      </c>
       <c r="F47" s="15" t="s">
         <v>329</v>
       </c>
@@ -13540,13 +14216,12 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>471</v>
+        <v>393</v>
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>482</v>
-      </c>
-      <c r="E48" s="22"/>
+        <v>426</v>
+      </c>
       <c r="F48" s="15" t="s">
         <v>329</v>
       </c>
@@ -13562,13 +14237,12 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
-        <v>472</v>
+        <v>394</v>
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>483</v>
-      </c>
-      <c r="E49" s="22"/>
+        <v>427</v>
+      </c>
       <c r="F49" s="15" t="s">
         <v>329</v>
       </c>
@@ -13582,15 +14256,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>473</v>
+        <v>506</v>
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="E50" s="22"/>
+        <v>507</v>
+      </c>
       <c r="F50" s="15" t="s">
         <v>329</v>
       </c>
@@ -13606,13 +14279,12 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
-        <v>474</v>
+        <v>395</v>
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="E51" s="22"/>
+        <v>428</v>
+      </c>
       <c r="F51" s="15" t="s">
         <v>329</v>
       </c>
@@ -13628,11 +14300,11 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B52" s="21"/>
       <c r="D52" s="15" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="15" t="s">
@@ -13650,11 +14322,11 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="15" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="15" t="s">
@@ -13672,11 +14344,11 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="15" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="15" t="s">
@@ -13693,19 +14365,114 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="44" t="s">
+        <v>473</v>
+      </c>
       <c r="B55" s="21"/>
+      <c r="D55" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="E55" s="22"/>
+      <c r="F55" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G55" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="44" t="s">
+        <v>474</v>
+      </c>
       <c r="B56" s="21"/>
+      <c r="D56" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="E56" s="22"/>
+      <c r="F56" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G56" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="44" t="s">
+        <v>476</v>
+      </c>
       <c r="B57" s="21"/>
+      <c r="D57" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="E57" s="22"/>
+      <c r="F57" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G57" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="44" t="s">
+        <v>475</v>
+      </c>
       <c r="B58" s="21"/>
+      <c r="D58" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="E58" s="22"/>
+      <c r="F58" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G58" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="44" t="s">
+        <v>480</v>
+      </c>
       <c r="B59" s="21"/>
+      <c r="D59" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="E59" s="22"/>
+      <c r="F59" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G59" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="21"/>
@@ -13754,6 +14521,21 @@
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="21"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="21"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="21"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="21"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="21"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Model 1-spd ASHPs as 2-spd units to temporarily workaround an issue. Will revert when we've updated to OS 1.11.5.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -5244,7 +5244,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5372,7 +5372,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$6.72/hour</v>
+        <v>$1.68/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>202</v>
@@ -5535,14 +5535,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="E24" s="22"/>
     </row>

</xml_diff>

<commit_message>
Added Hot Water Fixtures. Updated measures.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="548">
   <si>
     <t>type</t>
   </si>
@@ -1663,6 +1663,21 @@
   </si>
   <si>
     <t>res_stock_reporting.hvac_setpoints</t>
+  </si>
+  <si>
+    <t>Hot Water Fixtures</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.hot_water_fixtures</t>
+  </si>
+  <si>
+    <t>Set Hot Water Fixtures</t>
+  </si>
+  <si>
+    <t>Hot Water Fixtures Sample Value</t>
+  </si>
+  <si>
+    <t>hot_water_fixtures.txt</t>
   </si>
 </sst>
 </file>
@@ -5880,10 +5895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z178"/>
+  <dimension ref="A1:Z181"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10580,7 +10595,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10629,7 +10644,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10656,7 +10671,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10700,7 +10715,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>521</v>
+        <v>538</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10749,7 +10764,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10776,7 +10791,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>522</v>
+        <v>539</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10820,7 +10835,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -10869,7 +10884,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10896,7 +10911,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -10940,7 +10955,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -10989,7 +11004,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -11016,7 +11031,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -11060,7 +11075,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11109,7 +11124,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11136,7 +11151,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11180,7 +11195,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>330</v>
+        <v>530</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11229,7 +11244,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>332</v>
+        <v>534</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11256,7 +11271,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>331</v>
+        <v>531</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11300,7 +11315,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11349,7 +11364,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11376,7 +11391,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11420,7 +11435,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11469,7 +11484,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11496,7 +11511,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11540,7 +11555,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11589,7 +11604,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11616,7 +11631,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11660,7 +11675,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11709,7 +11724,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11736,7 +11751,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -11780,7 +11795,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>503</v>
+        <v>348</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -11829,7 +11844,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>505</v>
+        <v>350</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11856,7 +11871,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>504</v>
+        <v>349</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -11900,7 +11915,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>351</v>
+        <v>503</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -11949,7 +11964,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>353</v>
+        <v>505</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11976,7 +11991,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>352</v>
+        <v>504</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -12020,7 +12035,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>449</v>
+        <v>351</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -12069,7 +12084,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>454</v>
+        <v>353</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12096,7 +12111,7 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>450</v>
+        <v>352</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12140,7 +12155,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12189,7 +12204,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12216,7 +12231,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12260,7 +12275,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12309,7 +12324,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12336,7 +12351,7 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12380,7 +12395,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>235</v>
@@ -12429,7 +12444,7 @@
       </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10" t="s">
-        <v>453</v>
+        <v>469</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="10"/>
@@ -12456,7 +12471,7 @@
       </c>
       <c r="C164" s="41"/>
       <c r="D164" s="41" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>237</v>
@@ -12500,7 +12515,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>235</v>
@@ -12549,7 +12564,7 @@
       </c>
       <c r="H166" s="10"/>
       <c r="I166" s="10" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="J166" s="10"/>
       <c r="K166" s="10"/>
@@ -12576,7 +12591,7 @@
       </c>
       <c r="C167" s="41"/>
       <c r="D167" s="41" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>237</v>
@@ -12620,7 +12635,7 @@
         <v>1</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>235</v>
@@ -12669,7 +12684,7 @@
       </c>
       <c r="H169" s="10"/>
       <c r="I169" s="10" t="s">
-        <v>479</v>
+        <v>457</v>
       </c>
       <c r="J169" s="10"/>
       <c r="K169" s="10"/>
@@ -12696,7 +12711,7 @@
       </c>
       <c r="C170" s="41"/>
       <c r="D170" s="41" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>237</v>
@@ -12740,7 +12755,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>458</v>
+        <v>477</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>235</v>
@@ -12789,7 +12804,7 @@
       </c>
       <c r="H172" s="10"/>
       <c r="I172" s="10" t="s">
-        <v>460</v>
+        <v>479</v>
       </c>
       <c r="J172" s="10"/>
       <c r="K172" s="10"/>
@@ -12816,7 +12831,7 @@
       </c>
       <c r="C173" s="41"/>
       <c r="D173" s="41" t="s">
-        <v>459</v>
+        <v>478</v>
       </c>
       <c r="E173" s="41" t="s">
         <v>237</v>
@@ -12860,7 +12875,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>235</v>
@@ -12909,7 +12924,7 @@
       </c>
       <c r="H175" s="10"/>
       <c r="I175" s="10" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="J175" s="10"/>
       <c r="K175" s="10"/>
@@ -12936,7 +12951,7 @@
       </c>
       <c r="C176" s="41"/>
       <c r="D176" s="41" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E176" s="41" t="s">
         <v>237</v>
@@ -12975,77 +12990,197 @@
       <c r="W176" s="41"/>
       <c r="X176" s="41"/>
     </row>
-    <row r="177" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A177" s="42" t="b">
+    <row r="177" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A177" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B177" s="42" t="s">
+      <c r="B177" s="40" t="s">
+        <v>461</v>
+      </c>
+      <c r="C177" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D177" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E177" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F177" s="40"/>
+      <c r="G177" s="40"/>
+      <c r="H177" s="40"/>
+      <c r="I177" s="40"/>
+      <c r="J177" s="40"/>
+      <c r="K177" s="40"/>
+      <c r="L177" s="40"/>
+      <c r="M177" s="40"/>
+      <c r="N177" s="40"/>
+      <c r="O177" s="40"/>
+      <c r="P177" s="40"/>
+      <c r="Q177" s="40"/>
+      <c r="R177" s="40"/>
+      <c r="S177" s="40"/>
+      <c r="T177" s="40"/>
+      <c r="U177" s="40"/>
+      <c r="V177" s="40"/>
+      <c r="W177" s="40"/>
+      <c r="X177" s="40"/>
+    </row>
+    <row r="178" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="10"/>
+      <c r="B178" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E178" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F178" s="10"/>
+      <c r="G178" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H178" s="10"/>
+      <c r="I178" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="J178" s="10"/>
+      <c r="K178" s="10"/>
+      <c r="L178" s="10"/>
+      <c r="M178" s="10"/>
+      <c r="N178" s="10"/>
+      <c r="O178" s="10"/>
+      <c r="P178" s="10"/>
+      <c r="Q178" s="10"/>
+      <c r="R178" s="10"/>
+      <c r="S178" s="10"/>
+      <c r="T178" s="10"/>
+      <c r="U178" s="10"/>
+      <c r="V178" s="10"/>
+      <c r="W178" s="10"/>
+      <c r="X178" s="10"/>
+      <c r="Y178" s="15"/>
+      <c r="Z178" s="15"/>
+    </row>
+    <row r="179" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A179" s="41"/>
+      <c r="B179" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C179" s="41"/>
+      <c r="D179" s="41" t="s">
+        <v>462</v>
+      </c>
+      <c r="E179" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F179" s="41"/>
+      <c r="G179" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H179" s="41"/>
+      <c r="I179" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J179" s="41"/>
+      <c r="K179" s="41">
+        <v>0</v>
+      </c>
+      <c r="L179" s="41">
+        <v>1</v>
+      </c>
+      <c r="M179" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N179" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O179" s="41"/>
+      <c r="P179" s="41"/>
+      <c r="Q179" s="41"/>
+      <c r="R179" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S179" s="41"/>
+      <c r="T179" s="41"/>
+      <c r="U179" s="41"/>
+      <c r="V179" s="41"/>
+      <c r="W179" s="41"/>
+      <c r="X179" s="41"/>
+    </row>
+    <row r="180" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A180" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B180" s="42" t="s">
         <v>327</v>
       </c>
-      <c r="C177" s="42" t="s">
+      <c r="C180" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="D177" s="42" t="s">
+      <c r="D180" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="E177" s="42" t="s">
+      <c r="E180" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="F177" s="42"/>
-      <c r="G177" s="42"/>
-      <c r="H177" s="43"/>
-      <c r="I177" s="43"/>
-      <c r="J177" s="42"/>
-      <c r="K177" s="42"/>
-      <c r="L177" s="42"/>
-      <c r="M177" s="42"/>
-      <c r="N177" s="42"/>
-      <c r="O177" s="42"/>
-      <c r="P177" s="42"/>
-      <c r="Q177" s="42"/>
-      <c r="R177" s="42"/>
-      <c r="S177" s="42"/>
-      <c r="T177" s="42"/>
-      <c r="U177" s="42"/>
-      <c r="V177" s="42"/>
-      <c r="W177" s="42"/>
-      <c r="X177" s="42"/>
-    </row>
-    <row r="178" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A178" s="42" t="b">
+      <c r="F180" s="42"/>
+      <c r="G180" s="42"/>
+      <c r="H180" s="43"/>
+      <c r="I180" s="43"/>
+      <c r="J180" s="42"/>
+      <c r="K180" s="42"/>
+      <c r="L180" s="42"/>
+      <c r="M180" s="42"/>
+      <c r="N180" s="42"/>
+      <c r="O180" s="42"/>
+      <c r="P180" s="42"/>
+      <c r="Q180" s="42"/>
+      <c r="R180" s="42"/>
+      <c r="S180" s="42"/>
+      <c r="T180" s="42"/>
+      <c r="U180" s="42"/>
+      <c r="V180" s="42"/>
+      <c r="W180" s="42"/>
+      <c r="X180" s="42"/>
+    </row>
+    <row r="181" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A181" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B178" s="42" t="s">
+      <c r="B181" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C178" s="42" t="s">
+      <c r="C181" s="42" t="s">
         <v>512</v>
       </c>
-      <c r="D178" s="42" t="s">
+      <c r="D181" s="42" t="s">
         <v>512</v>
       </c>
-      <c r="E178" s="42" t="s">
+      <c r="E181" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="F178" s="42"/>
-      <c r="G178" s="42"/>
-      <c r="H178" s="43"/>
-      <c r="I178" s="43"/>
-      <c r="J178" s="42"/>
-      <c r="K178" s="42"/>
-      <c r="L178" s="42"/>
-      <c r="M178" s="42"/>
-      <c r="N178" s="42"/>
-      <c r="O178" s="42"/>
-      <c r="P178" s="42"/>
-      <c r="Q178" s="42"/>
-      <c r="R178" s="42"/>
-      <c r="S178" s="42"/>
-      <c r="T178" s="42"/>
-      <c r="U178" s="42"/>
-      <c r="V178" s="42"/>
-      <c r="W178" s="42"/>
-      <c r="X178" s="42"/>
+      <c r="F181" s="42"/>
+      <c r="G181" s="42"/>
+      <c r="H181" s="43"/>
+      <c r="I181" s="43"/>
+      <c r="J181" s="42"/>
+      <c r="K181" s="42"/>
+      <c r="L181" s="42"/>
+      <c r="M181" s="42"/>
+      <c r="N181" s="42"/>
+      <c r="O181" s="42"/>
+      <c r="P181" s="42"/>
+      <c r="Q181" s="42"/>
+      <c r="R181" s="42"/>
+      <c r="S181" s="42"/>
+      <c r="T181" s="42"/>
+      <c r="U181" s="42"/>
+      <c r="V181" s="42"/>
+      <c r="W181" s="42"/>
+      <c r="X181" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -13064,10 +13199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -14048,11 +14183,11 @@
     </row>
     <row r="40" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>329</v>
@@ -14069,11 +14204,11 @@
     </row>
     <row r="41" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="s">
-        <v>524</v>
+        <v>541</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>525</v>
+        <v>542</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>329</v>
@@ -14090,11 +14225,11 @@
     </row>
     <row r="42" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>329</v>
@@ -14111,11 +14246,11 @@
     </row>
     <row r="43" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>329</v>
@@ -14132,11 +14267,11 @@
     </row>
     <row r="44" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>329</v>
@@ -14151,13 +14286,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>390</v>
+        <v>527</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>397</v>
+        <v>535</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>329</v>
@@ -14174,11 +14309,11 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>329</v>
@@ -14195,11 +14330,11 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>398</v>
+        <v>425</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>329</v>
@@ -14216,11 +14351,11 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>426</v>
+        <v>398</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>329</v>
@@ -14237,11 +14372,11 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F49" s="15" t="s">
         <v>329</v>
@@ -14256,13 +14391,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>506</v>
+        <v>394</v>
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>507</v>
+        <v>427</v>
       </c>
       <c r="F50" s="15" t="s">
         <v>329</v>
@@ -14277,13 +14412,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
-        <v>395</v>
+        <v>506</v>
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>428</v>
+        <v>507</v>
       </c>
       <c r="F51" s="15" t="s">
         <v>329</v>
@@ -14300,13 +14435,12 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>470</v>
+        <v>395</v>
       </c>
       <c r="B52" s="21"/>
       <c r="D52" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="E52" s="22"/>
+        <v>428</v>
+      </c>
       <c r="F52" s="15" t="s">
         <v>329</v>
       </c>
@@ -14322,11 +14456,11 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="44" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="15" t="s">
@@ -14344,11 +14478,11 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="15" t="s">
@@ -14366,11 +14500,11 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B55" s="21"/>
       <c r="D55" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="15" t="s">
@@ -14388,11 +14522,11 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B56" s="21"/>
       <c r="D56" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E56" s="22"/>
       <c r="F56" s="15" t="s">
@@ -14410,11 +14544,11 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B57" s="21"/>
       <c r="D57" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="15" t="s">
@@ -14432,11 +14566,11 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B58" s="21"/>
       <c r="D58" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E58" s="22"/>
       <c r="F58" s="15" t="s">
@@ -14454,11 +14588,11 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B59" s="21"/>
       <c r="D59" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="15" t="s">
@@ -14475,7 +14609,26 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="44" t="s">
+        <v>480</v>
+      </c>
       <c r="B60" s="21"/>
+      <c r="D60" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="E60" s="22"/>
+      <c r="F60" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G60" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="21"/>
@@ -14536,6 +14689,9 @@
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="21"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Removed ParameterName header in probability distributions; using file names instead. Changed to tsv files.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -753,12 +753,6 @@
     <t>probability_file</t>
   </si>
   <si>
-    <t>vintage.txt</t>
-  </si>
-  <si>
-    <t>insulation_wall.txt</t>
-  </si>
-  <si>
     <t>Set Vintage</t>
   </si>
   <si>
@@ -777,18 +771,12 @@
     <t>../seeds/EmptySeedModel.osm</t>
   </si>
   <si>
-    <t>location_epw.txt</t>
-  </si>
-  <si>
     <t>Set Location EPW</t>
   </si>
   <si>
     <t>Set Location Region</t>
   </si>
   <si>
-    <t>location_region.txt</t>
-  </si>
-  <si>
     <t>Probability Distributions File</t>
   </si>
   <si>
@@ -801,33 +789,12 @@
     <t>Vintage Sample Value</t>
   </si>
   <si>
-    <t>geometry_foundation_type.txt</t>
-  </si>
-  <si>
-    <t>geometry_size.txt</t>
-  </si>
-  <si>
-    <t>geometry_stories.txt</t>
-  </si>
-  <si>
-    <t>geometry_garage.txt</t>
-  </si>
-  <si>
     <t>Set Geometry</t>
   </si>
   <si>
     <t>Geometry Sample Value</t>
   </si>
   <si>
-    <t>geometry.txt</t>
-  </si>
-  <si>
-    <t>Set Insulation Walls</t>
-  </si>
-  <si>
-    <t>Insulation Walls Sample Value</t>
-  </si>
-  <si>
     <t>Set Geometry Garage</t>
   </si>
   <si>
@@ -852,168 +819,72 @@
     <t>Geometry Foundation Type Sample Value</t>
   </si>
   <si>
-    <t>Set Insulation Walls Interzonal</t>
-  </si>
-  <si>
-    <t>Insulation Walls Interzonal Sample Value</t>
-  </si>
-  <si>
-    <t>insulation_wall_interzonal.txt</t>
-  </si>
-  <si>
     <t>Set Insulation Slab</t>
   </si>
   <si>
     <t>Insulation Slab Sample Value</t>
   </si>
   <si>
-    <t>insulation_slab.txt</t>
-  </si>
-  <si>
-    <t>Set Insulation Crawl</t>
-  </si>
-  <si>
-    <t>Insulation Crawl Sample Value</t>
-  </si>
-  <si>
-    <t>insulation_crawlspace.txt</t>
-  </si>
-  <si>
     <t>Set Insulation Unfinished Basement</t>
   </si>
   <si>
     <t>Insulation Unfinished Basement Sample Value</t>
   </si>
   <si>
-    <t>insulation_basement_unfinished.txt</t>
-  </si>
-  <si>
     <t>Set Insulation Finished Basement</t>
   </si>
   <si>
     <t>Insulation Finished Basement Sample Value</t>
   </si>
   <si>
-    <t>insulation_basement_finished.txt</t>
-  </si>
-  <si>
-    <t>insulation_unfinished_attic.txt</t>
-  </si>
-  <si>
     <t>Set Insulation Unfinished Attic</t>
   </si>
   <si>
     <t>Insulation Unfinished Attic Sample Value</t>
   </si>
   <si>
-    <t>Insulation Floors Interzonal Sample Value</t>
-  </si>
-  <si>
-    <t>Set Insulation Floors Interzonal</t>
-  </si>
-  <si>
-    <t>insulation_floor_interzonal.txt</t>
-  </si>
-  <si>
     <t>Set Wall Sheathing</t>
   </si>
   <si>
     <t>Wall Sheathing Sample Value</t>
   </si>
   <si>
-    <t>wall_sheathing.txt</t>
-  </si>
-  <si>
     <t>Set Exterior Finish</t>
   </si>
   <si>
     <t>Exterior Finish Sample Value</t>
   </si>
   <si>
-    <t>exterior_finish.txt</t>
-  </si>
-  <si>
     <t>Set Roof Material</t>
   </si>
   <si>
     <t>Roof Material Sample Value</t>
   </si>
   <si>
-    <t>roof_material.txt</t>
-  </si>
-  <si>
     <t>Set Floor Covering</t>
   </si>
   <si>
     <t>Floor Covering Sample Value</t>
   </si>
   <si>
-    <t>floor_covering.txt</t>
-  </si>
-  <si>
-    <t>Set Floor Mass</t>
-  </si>
-  <si>
-    <t>Floor Mass Sample Value</t>
-  </si>
-  <si>
-    <t>mass_floor.txt</t>
-  </si>
-  <si>
-    <t>Set Exterior Wall Mass</t>
-  </si>
-  <si>
-    <t>Exterior Wall Mass Sample Value</t>
-  </si>
-  <si>
-    <t>mass_exterior_wall.txt</t>
-  </si>
-  <si>
-    <t>Set Partition Wall Mass</t>
-  </si>
-  <si>
-    <t>Partition Wall Mass Sample Value</t>
-  </si>
-  <si>
-    <t>mass_partition_wall.txt</t>
-  </si>
-  <si>
-    <t>Set Ceiling Mass</t>
-  </si>
-  <si>
-    <t>Ceiling Mass Sample Value</t>
-  </si>
-  <si>
-    <t>mass_ceiling.txt</t>
-  </si>
-  <si>
     <t>Set Orientation</t>
   </si>
   <si>
     <t>Orientation Sample Value</t>
   </si>
   <si>
-    <t>orientation.txt</t>
-  </si>
-  <si>
     <t>Set Door Area</t>
   </si>
   <si>
     <t>Door Area Sample Value</t>
   </si>
   <si>
-    <t>door_area.txt</t>
-  </si>
-  <si>
     <t>Set Doors</t>
   </si>
   <si>
     <t>Doors Sample Value</t>
   </si>
   <si>
-    <t>doors.txt</t>
-  </si>
-  <si>
     <t>ReportingMeasure</t>
   </si>
   <si>
@@ -1032,81 +903,54 @@
     <t>Refrigerator Sample Value</t>
   </si>
   <si>
-    <t>refrigerator.txt</t>
-  </si>
-  <si>
     <t>Set Usage Level</t>
   </si>
   <si>
     <t>Usage Level Sample Value</t>
   </si>
   <si>
-    <t>usage_level.txt</t>
-  </si>
-  <si>
     <t>Set Cooking Range</t>
   </si>
   <si>
     <t>Cooking Range Sample Value</t>
   </si>
   <si>
-    <t>cooking_range.txt</t>
-  </si>
-  <si>
     <t>Set Heating Fuel</t>
   </si>
   <si>
     <t>Heating Fuel Sample Value</t>
   </si>
   <si>
-    <t>heating_fuel.txt</t>
-  </si>
-  <si>
     <t>Set Dishwasher</t>
   </si>
   <si>
     <t>Dishwasher Sample Value</t>
   </si>
   <si>
-    <t>dishwasher.txt</t>
-  </si>
-  <si>
     <t>Set Clothes Washer</t>
   </si>
   <si>
     <t>Clothes Washer Sample Value</t>
   </si>
   <si>
-    <t>clothes_washer.txt</t>
-  </si>
-  <si>
     <t>Set Clothes Dryer</t>
   </si>
   <si>
     <t>Clothes Dryer Sample Value</t>
   </si>
   <si>
-    <t>clothes_dryer.txt</t>
-  </si>
-  <si>
     <t>Set Plug Loads</t>
   </si>
   <si>
     <t>Plug Loads Sample Value</t>
   </si>
   <si>
-    <t>plug_loads.txt</t>
-  </si>
-  <si>
     <t>Set Water Heater</t>
   </si>
   <si>
     <t>Water Heater Sample Value</t>
   </si>
   <si>
-    <t>water_heater.txt</t>
-  </si>
-  <si>
     <t>Location Region</t>
   </si>
   <si>
@@ -1116,63 +960,30 @@
     <t>Vintage</t>
   </si>
   <si>
-    <t>res_stock_reporting.vintage</t>
-  </si>
-  <si>
     <t>Heating Fuel</t>
   </si>
   <si>
     <t>Usage Level</t>
   </si>
   <si>
-    <t>Foundation Type</t>
-  </si>
-  <si>
-    <t>House Size</t>
-  </si>
-  <si>
-    <t>Stories</t>
-  </si>
-  <si>
-    <t>Garage</t>
-  </si>
-  <si>
     <t>Geometry</t>
   </si>
   <si>
-    <t>res_stock_reporting.geometry</t>
-  </si>
-  <si>
     <t>Orientation</t>
   </si>
   <si>
-    <t>res_stock_reporting.orientation</t>
-  </si>
-  <si>
     <t>Insulation Unfinished Attic</t>
   </si>
   <si>
-    <t>Insulation Walls</t>
-  </si>
-  <si>
-    <t>Insulation Walls Interzonal</t>
-  </si>
-  <si>
     <t>Insulation Slab</t>
   </si>
   <si>
-    <t>Insulation Crawl</t>
-  </si>
-  <si>
     <t>Insulation Unfinished Basement</t>
   </si>
   <si>
     <t>Insulation Finished Basement</t>
   </si>
   <si>
-    <t>Insulation Floors Interzonal</t>
-  </si>
-  <si>
     <t>Wall Sheathing</t>
   </si>
   <si>
@@ -1185,18 +996,6 @@
     <t>Floor Covering</t>
   </si>
   <si>
-    <t>Floor Mass</t>
-  </si>
-  <si>
-    <t>Exterior Wall Mass</t>
-  </si>
-  <si>
-    <t>Partition Wall Mass</t>
-  </si>
-  <si>
-    <t>Ceiling Mass</t>
-  </si>
-  <si>
     <t>Door Area</t>
   </si>
   <si>
@@ -1224,315 +1023,60 @@
     <t>Plug Loads</t>
   </si>
   <si>
-    <t>res_stock_reporting.doors</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.refrigerator</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.dishwasher</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.location_region</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.location_epw</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.heating_fuel</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.usage_level</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.geometry_foundation_type</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.geometry_size</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.geometry_stories</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.geometry_garage</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_unfinished_attic</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_wall</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_wall_interzonal</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_slab</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_crawlspace</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_basement_unfinished</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_basement_finished</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.insulation_floor_interzonal</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.wall_sheathing</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.exterior_finish</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.roof_material</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.floor_covering</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.mass_floor</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.mass_exterior_wall</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.mass_partition_wall</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.mass_ceiling</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.door_area</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.water_heater</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.cooking_range</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.clothes_washer</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.clothes_dryer</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.plug_loads</t>
-  </si>
-  <si>
     <t>Set Neighbors</t>
   </si>
   <si>
     <t>Neighbors Sample Value</t>
   </si>
   <si>
-    <t>neighbors.txt</t>
-  </si>
-  <si>
     <t>Neighbors</t>
   </si>
   <si>
-    <t>res_stock_reporting.neighbors</t>
-  </si>
-  <si>
     <t>Set Eaves</t>
   </si>
   <si>
     <t>Eaves Sample Value</t>
   </si>
   <si>
-    <t>eaves.txt</t>
-  </si>
-  <si>
     <t>Eaves</t>
   </si>
   <si>
-    <t>res_stock_reporting.eaves</t>
-  </si>
-  <si>
     <t>Set Overhangs</t>
   </si>
   <si>
     <t>Overhangs Sample Value</t>
   </si>
   <si>
-    <t>overhangs.txt</t>
-  </si>
-  <si>
     <t>Overhangs</t>
   </si>
   <si>
-    <t>res_stock_reporting.overhangs</t>
-  </si>
-  <si>
     <t>Set Uninsulated Surfaces</t>
   </si>
   <si>
     <t>Uninsulated Surfaces Sample Value</t>
   </si>
   <si>
-    <t>uninsulated_surfaces.txt</t>
-  </si>
-  <si>
     <t>Uninsulated Surfaces</t>
   </si>
   <si>
-    <t>res_stock_reporting.uninsulated_surfaces</t>
-  </si>
-  <si>
-    <t>Set Extra Refrigerator</t>
-  </si>
-  <si>
-    <t>Extra Refrigerator Sample Value</t>
-  </si>
-  <si>
-    <t>Set Gas Grill</t>
-  </si>
-  <si>
-    <t>Gas Grill Sample Value</t>
-  </si>
-  <si>
-    <t>misc_gas_grill.txt</t>
-  </si>
-  <si>
-    <t>misc_extra_refrigerator.txt</t>
-  </si>
-  <si>
-    <t>Set Gas Lighting</t>
-  </si>
-  <si>
-    <t>Gas Lighting Sample Value</t>
-  </si>
-  <si>
-    <t>misc_gas_lighting.txt</t>
-  </si>
-  <si>
-    <t>Set Pool</t>
-  </si>
-  <si>
-    <t>Pool Sample Value</t>
-  </si>
-  <si>
-    <t>misc_pool.txt</t>
-  </si>
-  <si>
-    <t>Set Well Pump</t>
-  </si>
-  <si>
-    <t>Well Pump Sample Value</t>
-  </si>
-  <si>
-    <t>misc_well_pump.txt</t>
-  </si>
-  <si>
-    <t>Set Freezer</t>
-  </si>
-  <si>
-    <t>Freezer Sample Value</t>
-  </si>
-  <si>
-    <t>misc_freezer.txt</t>
-  </si>
-  <si>
-    <t>Set Gas Fireplace</t>
-  </si>
-  <si>
-    <t>Gas Fireplace Sample Value</t>
-  </si>
-  <si>
-    <t>misc_gas_fireplace.txt</t>
-  </si>
-  <si>
-    <t>Extra Refrigerator</t>
-  </si>
-  <si>
-    <t>Freezer</t>
-  </si>
-  <si>
-    <t>Gas Fireplace</t>
-  </si>
-  <si>
-    <t>Gas Grill</t>
-  </si>
-  <si>
-    <t>Gas Lighting</t>
-  </si>
-  <si>
-    <t>Pool</t>
-  </si>
-  <si>
-    <t>Hot Tub/Spa</t>
-  </si>
-  <si>
-    <t>Set Hot Tub/Spa</t>
-  </si>
-  <si>
-    <t>Hot Tub/Spa Sample Value</t>
-  </si>
-  <si>
-    <t>misc_hot_tub_spa.txt</t>
-  </si>
-  <si>
-    <t>Well Pump</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_extra_refrigerator</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_freezer</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_gas_fireplace</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_gas_grill</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_gas_lighting</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_hot_tub_spa</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_pool</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.misc_well_pump</t>
-  </si>
-  <si>
     <t>Window Areas</t>
   </si>
   <si>
-    <t>res_stock_reporting.window_areas</t>
-  </si>
-  <si>
     <t>Set Window Areas</t>
   </si>
   <si>
     <t>Window Areas Sample Value</t>
   </si>
   <si>
-    <t>window_areas.txt</t>
-  </si>
-  <si>
     <t>Set Windows</t>
   </si>
   <si>
     <t>Windows Sample Value</t>
   </si>
   <si>
-    <t>windows.txt</t>
-  </si>
-  <si>
     <t>Windows</t>
   </si>
   <si>
-    <t>res_stock_reporting.windows</t>
-  </si>
-  <si>
     <t>../results/pnw</t>
   </si>
   <si>
@@ -1551,27 +1095,12 @@
     <t>Lighting Sample Value</t>
   </si>
   <si>
-    <t>lighting.txt</t>
-  </si>
-  <si>
     <t>Lighting</t>
   </si>
   <si>
-    <t>res_stock_reporting.lighting</t>
-  </si>
-  <si>
     <t>1.15.7-resstock</t>
   </si>
   <si>
-    <t>Set Insulation Pier &amp; Beam</t>
-  </si>
-  <si>
-    <t>insulation_pier_beam.txt</t>
-  </si>
-  <si>
-    <t>Insulation Pier &amp; Beam Sample Value</t>
-  </si>
-  <si>
     <t>ServerDirectoryCleanup</t>
   </si>
   <si>
@@ -1590,9 +1119,6 @@
     <t>../weather/pnw/*.*</t>
   </si>
   <si>
-    <t>hvac_system_combined.txt</t>
-  </si>
-  <si>
     <t>Set HVAC System Combined</t>
   </si>
   <si>
@@ -1605,15 +1131,9 @@
     <t>HVAC System Is Combined Sample Value</t>
   </si>
   <si>
-    <t>hvac_system_is_combined.txt</t>
-  </si>
-  <si>
     <t>HVAC System Is Combined</t>
   </si>
   <si>
-    <t>res_stock_reporting.hvac_system_is_combined</t>
-  </si>
-  <si>
     <t>HVAC System Combined</t>
   </si>
   <si>
@@ -1635,49 +1155,529 @@
     <t>HVAC System Heating Sample Value</t>
   </si>
   <si>
-    <t>hvac_system_heating.txt</t>
-  </si>
-  <si>
-    <t>hvac_system_cooling.txt</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.hvac_system_cooling</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.hvac_system_heating</t>
-  </si>
-  <si>
-    <t>res_stock_reporting.hvac_system_combined</t>
-  </si>
-  <si>
     <t>Set HVAC Setpoints</t>
   </si>
   <si>
     <t>HVAC Setpoints Sample Value</t>
   </si>
   <si>
-    <t>hvac_setpoints.txt</t>
-  </si>
-  <si>
     <t>HVAC Setpoints</t>
   </si>
   <si>
-    <t>res_stock_reporting.hvac_setpoints</t>
-  </si>
-  <si>
     <t>Hot Water Fixtures</t>
   </si>
   <si>
-    <t>res_stock_reporting.hot_water_fixtures</t>
-  </si>
-  <si>
     <t>Set Hot Water Fixtures</t>
   </si>
   <si>
     <t>Hot Water Fixtures Sample Value</t>
   </si>
   <si>
-    <t>hot_water_fixtures.txt</t>
+    <t>Clothes Dryer.tsv</t>
+  </si>
+  <si>
+    <t>Clothes Washer.tsv</t>
+  </si>
+  <si>
+    <t>Cooking Range.tsv</t>
+  </si>
+  <si>
+    <t>Dishwasher.tsv</t>
+  </si>
+  <si>
+    <t>Door Area.tsv</t>
+  </si>
+  <si>
+    <t>Doors.tsv</t>
+  </si>
+  <si>
+    <t>Eaves.tsv</t>
+  </si>
+  <si>
+    <t>Exterior Finish.tsv</t>
+  </si>
+  <si>
+    <t>Floor Covering.tsv</t>
+  </si>
+  <si>
+    <t>Geometry Foundation Type.tsv</t>
+  </si>
+  <si>
+    <t>Geometry Garage.tsv</t>
+  </si>
+  <si>
+    <t>Geometry House Size.tsv</t>
+  </si>
+  <si>
+    <t>Geometry Stories.tsv</t>
+  </si>
+  <si>
+    <t>Geometry.tsv</t>
+  </si>
+  <si>
+    <t>Heating Fuel.tsv</t>
+  </si>
+  <si>
+    <t>Hot Water Fixtures.tsv</t>
+  </si>
+  <si>
+    <t>HVAC Setpoints.tsv</t>
+  </si>
+  <si>
+    <t>HVAC System Combined.tsv</t>
+  </si>
+  <si>
+    <t>HVAC System Cooling.tsv</t>
+  </si>
+  <si>
+    <t>HVAC System Heating.tsv</t>
+  </si>
+  <si>
+    <t>HVAC System Is Combined.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Crawlspace.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Finished Basement.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Interzonal Floor.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Interzonal Wall.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Slab.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Attic.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Basement.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Wall.tsv</t>
+  </si>
+  <si>
+    <t>Lighting.tsv</t>
+  </si>
+  <si>
+    <t>Location EPW.tsv</t>
+  </si>
+  <si>
+    <t>Location Region.tsv</t>
+  </si>
+  <si>
+    <t>Misc Extra Refrigerator.tsv</t>
+  </si>
+  <si>
+    <t>Misc Freezer.tsv</t>
+  </si>
+  <si>
+    <t>Misc Gas Fireplace.tsv</t>
+  </si>
+  <si>
+    <t>Misc Gas Grill.tsv</t>
+  </si>
+  <si>
+    <t>Misc Gas Lighting.tsv</t>
+  </si>
+  <si>
+    <t>Misc Hot Tub Spa.tsv</t>
+  </si>
+  <si>
+    <t>Misc Pool.tsv</t>
+  </si>
+  <si>
+    <t>Misc Well Pump.tsv</t>
+  </si>
+  <si>
+    <t>Neighbors.tsv</t>
+  </si>
+  <si>
+    <t>Orientation.tsv</t>
+  </si>
+  <si>
+    <t>Overhangs.tsv</t>
+  </si>
+  <si>
+    <t>Plug Loads.tsv</t>
+  </si>
+  <si>
+    <t>Refrigerator.tsv</t>
+  </si>
+  <si>
+    <t>Roof Material.tsv</t>
+  </si>
+  <si>
+    <t>Thermal Mass Ceiling.tsv</t>
+  </si>
+  <si>
+    <t>Thermal Mass Exterior Wall.tsv</t>
+  </si>
+  <si>
+    <t>Thermal Mass Floor.tsv</t>
+  </si>
+  <si>
+    <t>Thermal Mass Partition Wall.tsv</t>
+  </si>
+  <si>
+    <t>Uninsulated Surfaces.tsv</t>
+  </si>
+  <si>
+    <t>Usage Level.tsv</t>
+  </si>
+  <si>
+    <t>Vintage.tsv</t>
+  </si>
+  <si>
+    <t>Wall Sheathing.tsv</t>
+  </si>
+  <si>
+    <t>Water Heater.tsv</t>
+  </si>
+  <si>
+    <t>Window Areas.tsv</t>
+  </si>
+  <si>
+    <t>Windows.tsv</t>
+  </si>
+  <si>
+    <t>Insulation Pier Beam.tsv</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Location Region</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Clothes Dryer</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Clothes Washer</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Cooking Range</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Dishwasher</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Door Area</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Doors</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Eaves</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Exterior Finish</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Floor Covering</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Geometry Foundation Type</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Geometry Garage</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Geometry House Size</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Geometry Stories</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Geometry</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Heating Fuel</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Hot Water Fixtures</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.HVAC Setpoints</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.HVAC System Combined</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.HVAC System Cooling</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.HVAC System Heating</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.HVAC System Is Combined</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Crawlspace</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Finished Basement</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Interzonal Floor</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Interzonal Wall</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Slab</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Unfinished Attic</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Unfinished Basement</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Insulation Wall</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Lighting</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Location EPW</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Extra Refrigerator</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Freezer</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Gas Fireplace</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Gas Grill</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Gas Lighting</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Hot Tub Spa</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Pool</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Misc Well Pump</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Neighbors</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Orientation</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Overhangs</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Plug Loads</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Refrigerator</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Roof Material</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Thermal Mass Ceiling</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Thermal Mass Exterior Wall</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Thermal Mass Floor</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Thermal Mass Partition Wall</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Uninsulated Surfaces</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Usage Level</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Vintage</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Wall Sheathing</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Water Heater</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Window Areas</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Windows</t>
+  </si>
+  <si>
+    <t>Geometry Foundation Type</t>
+  </si>
+  <si>
+    <t>Geometry House Size</t>
+  </si>
+  <si>
+    <t>Geometry Stories</t>
+  </si>
+  <si>
+    <t>Geometry Garage</t>
+  </si>
+  <si>
+    <t>Insulation Wall</t>
+  </si>
+  <si>
+    <t>Insulation Interzonal Wall</t>
+  </si>
+  <si>
+    <t>Insulation Crawlspace</t>
+  </si>
+  <si>
+    <t>Insulation Interzonal Floor</t>
+  </si>
+  <si>
+    <t>Thermal Mass Floor</t>
+  </si>
+  <si>
+    <t>Thermal Mass Exterior Wall</t>
+  </si>
+  <si>
+    <t>Thermal Mass Partition Wall</t>
+  </si>
+  <si>
+    <t>Thermal Mass Ceiling</t>
+  </si>
+  <si>
+    <t>Misc Extra Refrigerator</t>
+  </si>
+  <si>
+    <t>Misc Freezer</t>
+  </si>
+  <si>
+    <t>Misc Gas Fireplace</t>
+  </si>
+  <si>
+    <t>Misc Gas Grill</t>
+  </si>
+  <si>
+    <t>Misc Gas Lighting</t>
+  </si>
+  <si>
+    <t>Misc Hot Tub Spa</t>
+  </si>
+  <si>
+    <t>Misc Pool</t>
+  </si>
+  <si>
+    <t>Misc Well Pump</t>
+  </si>
+  <si>
+    <t>Set Insulation Wall</t>
+  </si>
+  <si>
+    <t>Insulation Wall Sample Value</t>
+  </si>
+  <si>
+    <t>Set Insulation Interzonal Wall</t>
+  </si>
+  <si>
+    <t>Insulation Interzonal Wall Sample Value</t>
+  </si>
+  <si>
+    <t>Insulation Crawlspace Sample Value</t>
+  </si>
+  <si>
+    <t>Set Insulation Crawlspace</t>
+  </si>
+  <si>
+    <t>Set Insulation Pier Beam</t>
+  </si>
+  <si>
+    <t>Insulation Pier Beam Sample Value</t>
+  </si>
+  <si>
+    <t>Set Insulation Interzonal Floor</t>
+  </si>
+  <si>
+    <t>Insulation Interzonal Floor Sample Value</t>
+  </si>
+  <si>
+    <t>Set Thermal Mass Floor</t>
+  </si>
+  <si>
+    <t>Thermal Mass Floor Sample Value</t>
+  </si>
+  <si>
+    <t>Set Thermal Mass Exterior Wall</t>
+  </si>
+  <si>
+    <t>Thermal Mass Exterior Wall Sample Value</t>
+  </si>
+  <si>
+    <t>Set Thermal Mass Partition Wall</t>
+  </si>
+  <si>
+    <t>Thermal Mass Partition Wall Sample Value</t>
+  </si>
+  <si>
+    <t>Set Thermal Mass Ceiling</t>
+  </si>
+  <si>
+    <t>Thermal Mass Ceiling Sample Value</t>
+  </si>
+  <si>
+    <t>Misc Extra Refrigerator Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Extra Refrigerator</t>
+  </si>
+  <si>
+    <t>Set Misc Freezer</t>
+  </si>
+  <si>
+    <t>Misc Freezer Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Gas Fireplace</t>
+  </si>
+  <si>
+    <t>Misc Gas Fireplace Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Gas Grill</t>
+  </si>
+  <si>
+    <t>Misc Gas Grill Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Gas Lighting</t>
+  </si>
+  <si>
+    <t>Misc Gas Lighting Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Hot Tub Spa</t>
+  </si>
+  <si>
+    <t>Misc Hot Tub Spa Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Pool</t>
+  </si>
+  <si>
+    <t>Misc Pool Sample Value</t>
+  </si>
+  <si>
+    <t>Set Misc Well Pump</t>
+  </si>
+  <si>
+    <t>Misc Well Pump Sample Value</t>
   </si>
 </sst>
 </file>
@@ -3354,7 +3354,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3441,7 +3441,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5258,8 +5257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5318,8 +5317,8 @@
       <c r="A5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>508</v>
+      <c r="B5" s="44" t="s">
+        <v>354</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
@@ -5340,7 +5339,7 @@
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="45" t="s">
         <v>147</v>
       </c>
       <c r="C7" s="23" t="str">
@@ -5387,7 +5386,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5395,7 +5394,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$1.68/hour</v>
+        <v>$6.72/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>202</v>
@@ -5430,7 +5429,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>500</v>
+        <v>348</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>77</v>
@@ -5441,7 +5440,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>156</v>
@@ -5452,7 +5451,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>499</v>
+        <v>347</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>156</v>
@@ -5550,14 +5549,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="E24" s="22"/>
     </row>
@@ -5765,7 +5764,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>517</v>
+        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5797,7 +5796,7 @@
         <v>38</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>58</v>
@@ -5820,14 +5819,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="48" t="s">
-        <v>514</v>
+      <c r="A44" s="47" t="s">
+        <v>357</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>515</v>
+        <v>358</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>516</v>
+        <v>359</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -5897,9 +5896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z181"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5953,14 +5950,14 @@
       <c r="R1" s="30"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -6081,13 +6078,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>502</v>
+        <v>350</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>41</v>
@@ -6119,10 +6116,10 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
@@ -6130,7 +6127,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>501</v>
+        <v>349</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -6155,7 +6152,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C6" s="40" t="s">
         <v>235</v>
@@ -6193,7 +6190,7 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>238</v>
@@ -6204,7 +6201,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>250</v>
+        <v>410</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6231,7 +6228,7 @@
       </c>
       <c r="C8" s="41"/>
       <c r="D8" s="41" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>237</v>
@@ -6275,7 +6272,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C9" s="40" t="s">
         <v>235</v>
@@ -6313,7 +6310,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>238</v>
@@ -6324,7 +6321,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>247</v>
+        <v>409</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6351,7 +6348,7 @@
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E11" s="41" t="s">
         <v>237</v>
@@ -6395,7 +6392,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C12" s="40" t="s">
         <v>235</v>
@@ -6433,7 +6430,7 @@
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>238</v>
@@ -6444,7 +6441,7 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>239</v>
+        <v>431</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -6471,7 +6468,7 @@
       </c>
       <c r="C14" s="41"/>
       <c r="D14" s="41" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>237</v>
@@ -6515,7 +6512,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>339</v>
+        <v>293</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>235</v>
@@ -6553,7 +6550,7 @@
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>238</v>
@@ -6564,7 +6561,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6591,7 +6588,7 @@
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="41" t="s">
-        <v>340</v>
+        <v>294</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>237</v>
@@ -6635,7 +6632,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>333</v>
+        <v>289</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>235</v>
@@ -6673,7 +6670,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>238</v>
@@ -6684,7 +6681,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>335</v>
+        <v>430</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6711,7 +6708,7 @@
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="41" t="s">
-        <v>334</v>
+        <v>290</v>
       </c>
       <c r="E20" s="41" t="s">
         <v>237</v>
@@ -6755,7 +6752,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>235</v>
@@ -6793,7 +6790,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>238</v>
@@ -6804,7 +6801,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>255</v>
+        <v>388</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6831,7 +6828,7 @@
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>237</v>
@@ -6875,7 +6872,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>235</v>
@@ -6913,7 +6910,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>238</v>
@@ -6924,7 +6921,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>256</v>
+        <v>390</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -6951,7 +6948,7 @@
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="E26" s="41" t="s">
         <v>237</v>
@@ -6995,7 +6992,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>235</v>
@@ -7033,7 +7030,7 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>238</v>
@@ -7044,7 +7041,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>257</v>
+        <v>391</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -7071,7 +7068,7 @@
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="E29" s="41" t="s">
         <v>237</v>
@@ -7115,7 +7112,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>235</v>
@@ -7153,7 +7150,7 @@
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>238</v>
@@ -7164,7 +7161,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>258</v>
+        <v>389</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7191,7 +7188,7 @@
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E32" s="41" t="s">
         <v>237</v>
@@ -7235,7 +7232,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>235</v>
@@ -7273,7 +7270,7 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>238</v>
@@ -7284,7 +7281,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>261</v>
+        <v>392</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7311,7 +7308,7 @@
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="41" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>237</v>
@@ -7355,7 +7352,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>317</v>
+        <v>277</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>235</v>
@@ -7393,7 +7390,7 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>238</v>
@@ -7404,7 +7401,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>319</v>
+        <v>420</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7431,7 +7428,7 @@
       </c>
       <c r="C38" s="41"/>
       <c r="D38" s="41" t="s">
-        <v>318</v>
+        <v>278</v>
       </c>
       <c r="E38" s="41" t="s">
         <v>237</v>
@@ -7475,7 +7472,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>434</v>
+        <v>332</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>235</v>
@@ -7513,7 +7510,7 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>238</v>
@@ -7524,7 +7521,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>436</v>
+        <v>385</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7551,7 +7548,7 @@
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="41" t="s">
-        <v>435</v>
+        <v>333</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>237</v>
@@ -7595,7 +7592,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>439</v>
+        <v>335</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>235</v>
@@ -7633,7 +7630,7 @@
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>238</v>
@@ -7644,7 +7641,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7671,7 +7668,7 @@
       </c>
       <c r="C44" s="41"/>
       <c r="D44" s="41" t="s">
-        <v>440</v>
+        <v>336</v>
       </c>
       <c r="E44" s="41" t="s">
         <v>237</v>
@@ -7715,7 +7712,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>235</v>
@@ -7753,7 +7750,7 @@
       </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>238</v>
@@ -7764,7 +7761,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>322</v>
+        <v>383</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7791,7 +7788,7 @@
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="41" t="s">
-        <v>321</v>
+        <v>280</v>
       </c>
       <c r="E47" s="41" t="s">
         <v>237</v>
@@ -7835,7 +7832,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>491</v>
+        <v>342</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>235</v>
@@ -7873,7 +7870,7 @@
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>238</v>
@@ -7884,7 +7881,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>493</v>
+        <v>434</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -7911,7 +7908,7 @@
       </c>
       <c r="C50" s="41"/>
       <c r="D50" s="41" t="s">
-        <v>492</v>
+        <v>343</v>
       </c>
       <c r="E50" s="41" t="s">
         <v>237</v>
@@ -7955,7 +7952,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>429</v>
+        <v>329</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>235</v>
@@ -7993,7 +7990,7 @@
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>238</v>
@@ -8004,7 +8001,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -8031,7 +8028,7 @@
       </c>
       <c r="C53" s="41"/>
       <c r="D53" s="41" t="s">
-        <v>430</v>
+        <v>330</v>
       </c>
       <c r="E53" s="41" t="s">
         <v>237</v>
@@ -8075,7 +8072,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>235</v>
@@ -8113,7 +8110,7 @@
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>238</v>
@@ -8124,7 +8121,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>287</v>
+        <v>405</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8151,7 +8148,7 @@
       </c>
       <c r="C56" s="41"/>
       <c r="D56" s="41" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="E56" s="41" t="s">
         <v>237</v>
@@ -8195,7 +8192,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>262</v>
+        <v>514</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>235</v>
@@ -8233,7 +8230,7 @@
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>238</v>
@@ -8244,7 +8241,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>240</v>
+        <v>407</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8271,7 +8268,7 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41" t="s">
-        <v>263</v>
+        <v>515</v>
       </c>
       <c r="E59" s="41" t="s">
         <v>237</v>
@@ -8315,7 +8312,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>272</v>
+        <v>516</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>235</v>
@@ -8353,7 +8350,7 @@
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>238</v>
@@ -8364,7 +8361,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>274</v>
+        <v>403</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8391,7 +8388,7 @@
       </c>
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>273</v>
+        <v>517</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>237</v>
@@ -8435,7 +8432,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="C63" s="40" t="s">
         <v>235</v>
@@ -8473,7 +8470,7 @@
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>238</v>
@@ -8484,7 +8481,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>277</v>
+        <v>404</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8511,7 +8508,7 @@
       </c>
       <c r="C65" s="41"/>
       <c r="D65" s="41" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="E65" s="41" t="s">
         <v>237</v>
@@ -8555,7 +8552,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>278</v>
+        <v>519</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>235</v>
@@ -8593,7 +8590,7 @@
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>238</v>
@@ -8604,7 +8601,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>280</v>
+        <v>400</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8631,7 +8628,7 @@
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="41" t="s">
-        <v>279</v>
+        <v>518</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>237</v>
@@ -8675,7 +8672,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="C69" s="40" t="s">
         <v>235</v>
@@ -8713,7 +8710,7 @@
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>238</v>
@@ -8724,7 +8721,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>283</v>
+        <v>406</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8751,7 +8748,7 @@
       </c>
       <c r="C71" s="41"/>
       <c r="D71" s="41" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="E71" s="41" t="s">
         <v>237</v>
@@ -8795,7 +8792,7 @@
         <v>1</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="C72" s="40" t="s">
         <v>235</v>
@@ -8833,7 +8830,7 @@
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>238</v>
@@ -8844,7 +8841,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>286</v>
+        <v>401</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -8871,7 +8868,7 @@
       </c>
       <c r="C74" s="41"/>
       <c r="D74" s="41" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="E74" s="41" t="s">
         <v>237</v>
@@ -8911,11 +8908,11 @@
       <c r="X74" s="41"/>
     </row>
     <row r="75" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="47" t="b">
+      <c r="A75" s="46" t="b">
         <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="C75" s="40" t="s">
         <v>235</v>
@@ -8953,7 +8950,7 @@
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>238</v>
@@ -8964,7 +8961,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>510</v>
+        <v>436</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8991,7 +8988,7 @@
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>237</v>
@@ -9035,7 +9032,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>291</v>
+        <v>522</v>
       </c>
       <c r="C78" s="40" t="s">
         <v>235</v>
@@ -9073,7 +9070,7 @@
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>238</v>
@@ -9084,7 +9081,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>292</v>
+        <v>402</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -9111,7 +9108,7 @@
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41" t="s">
-        <v>290</v>
+        <v>523</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>237</v>
@@ -9155,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>444</v>
+        <v>338</v>
       </c>
       <c r="C81" s="40" t="s">
         <v>235</v>
@@ -9193,7 +9190,7 @@
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>238</v>
@@ -9204,7 +9201,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9231,7 +9228,7 @@
       </c>
       <c r="C83" s="41"/>
       <c r="D83" s="41" t="s">
-        <v>445</v>
+        <v>339</v>
       </c>
       <c r="E83" s="41" t="s">
         <v>237</v>
@@ -9275,7 +9272,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="C84" s="40" t="s">
         <v>235</v>
@@ -9313,7 +9310,7 @@
       </c>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>238</v>
@@ -9324,7 +9321,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>295</v>
+        <v>432</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9351,7 +9348,7 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="41" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>237</v>
@@ -9395,7 +9392,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="C87" s="40" t="s">
         <v>235</v>
@@ -9433,7 +9430,7 @@
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>238</v>
@@ -9444,7 +9441,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>298</v>
+        <v>386</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9471,7 +9468,7 @@
       </c>
       <c r="C89" s="41"/>
       <c r="D89" s="41" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>237</v>
@@ -9515,7 +9512,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>299</v>
+        <v>273</v>
       </c>
       <c r="C90" s="40" t="s">
         <v>235</v>
@@ -9553,7 +9550,7 @@
       </c>
       <c r="C91" s="10"/>
       <c r="D91" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>238</v>
@@ -9564,7 +9561,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>301</v>
+        <v>424</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9591,7 +9588,7 @@
       </c>
       <c r="C92" s="41"/>
       <c r="D92" s="41" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="E92" s="41" t="s">
         <v>237</v>
@@ -9635,7 +9632,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
       <c r="C93" s="40" t="s">
         <v>235</v>
@@ -9673,7 +9670,7 @@
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>238</v>
@@ -9684,7 +9681,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>304</v>
+        <v>387</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9711,7 +9708,7 @@
       </c>
       <c r="C95" s="41"/>
       <c r="D95" s="41" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="E95" s="41" t="s">
         <v>237</v>
@@ -9755,7 +9752,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>305</v>
+        <v>524</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>235</v>
@@ -9793,7 +9790,7 @@
       </c>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>238</v>
@@ -9804,7 +9801,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>307</v>
+        <v>427</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9831,7 +9828,7 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>306</v>
+        <v>525</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>237</v>
@@ -9875,7 +9872,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>308</v>
+        <v>526</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>235</v>
@@ -9913,7 +9910,7 @@
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E100" s="10" t="s">
         <v>238</v>
@@ -9924,7 +9921,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>310</v>
+        <v>426</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9951,7 +9948,7 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>309</v>
+        <v>527</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>237</v>
@@ -9995,7 +9992,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>311</v>
+        <v>528</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>235</v>
@@ -10033,7 +10030,7 @@
       </c>
       <c r="C103" s="10"/>
       <c r="D103" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>238</v>
@@ -10044,7 +10041,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>313</v>
+        <v>428</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -10071,7 +10068,7 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>312</v>
+        <v>529</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>237</v>
@@ -10115,7 +10112,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>314</v>
+        <v>530</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>235</v>
@@ -10153,7 +10150,7 @@
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E106" s="10" t="s">
         <v>238</v>
@@ -10164,7 +10161,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>316</v>
+        <v>425</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10191,7 +10188,7 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>315</v>
+        <v>531</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>237</v>
@@ -10235,7 +10232,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>323</v>
+        <v>281</v>
       </c>
       <c r="C108" s="40" t="s">
         <v>235</v>
@@ -10273,7 +10270,7 @@
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E109" s="10" t="s">
         <v>238</v>
@@ -10284,7 +10281,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>325</v>
+        <v>384</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10311,7 +10308,7 @@
       </c>
       <c r="C110" s="41"/>
       <c r="D110" s="41" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="E110" s="41" t="s">
         <v>237</v>
@@ -10355,7 +10352,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>494</v>
+        <v>344</v>
       </c>
       <c r="C111" s="40" t="s">
         <v>235</v>
@@ -10393,7 +10390,7 @@
       </c>
       <c r="C112" s="10"/>
       <c r="D112" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E112" s="10" t="s">
         <v>238</v>
@@ -10404,7 +10401,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>496</v>
+        <v>435</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10431,7 +10428,7 @@
       </c>
       <c r="C113" s="41"/>
       <c r="D113" s="41" t="s">
-        <v>495</v>
+        <v>345</v>
       </c>
       <c r="E113" s="41" t="s">
         <v>237</v>
@@ -10475,7 +10472,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>354</v>
+        <v>303</v>
       </c>
       <c r="C114" s="40" t="s">
         <v>235</v>
@@ -10513,7 +10510,7 @@
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>238</v>
@@ -10524,7 +10521,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>356</v>
+        <v>433</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10551,7 +10548,7 @@
       </c>
       <c r="C116" s="41"/>
       <c r="D116" s="41" t="s">
-        <v>355</v>
+        <v>304</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>237</v>
@@ -10595,7 +10592,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>545</v>
+        <v>377</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10633,7 +10630,7 @@
       </c>
       <c r="C118" s="10"/>
       <c r="D118" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E118" s="10" t="s">
         <v>238</v>
@@ -10644,7 +10641,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>547</v>
+        <v>394</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10671,7 +10668,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>546</v>
+        <v>378</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10715,7 +10712,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>538</v>
+        <v>373</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10753,7 +10750,7 @@
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E121" s="10" t="s">
         <v>238</v>
@@ -10764,7 +10761,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>540</v>
+        <v>395</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10791,7 +10788,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>539</v>
+        <v>374</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10835,7 +10832,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>521</v>
+        <v>363</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -10873,7 +10870,7 @@
       </c>
       <c r="C124" s="10"/>
       <c r="D124" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E124" s="10" t="s">
         <v>238</v>
@@ -10884,7 +10881,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>523</v>
+        <v>399</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10911,7 +10908,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>522</v>
+        <v>364</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -10955,7 +10952,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>519</v>
+        <v>361</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -10993,7 +10990,7 @@
       </c>
       <c r="C127" s="10"/>
       <c r="D127" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E127" s="10" t="s">
         <v>238</v>
@@ -11004,7 +11001,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>518</v>
+        <v>396</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -11031,7 +11028,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>520</v>
+        <v>362</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -11075,7 +11072,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>529</v>
+        <v>369</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11113,7 +11110,7 @@
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E130" s="10" t="s">
         <v>238</v>
@@ -11124,7 +11121,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>533</v>
+        <v>398</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11151,7 +11148,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>532</v>
+        <v>372</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11195,7 +11192,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>530</v>
+        <v>370</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11233,7 +11230,7 @@
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E133" s="10" t="s">
         <v>238</v>
@@ -11244,7 +11241,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>534</v>
+        <v>397</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11271,7 +11268,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>531</v>
+        <v>371</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11315,7 +11312,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11353,7 +11350,7 @@
       </c>
       <c r="C136" s="10"/>
       <c r="D136" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E136" s="10" t="s">
         <v>238</v>
@@ -11364,7 +11361,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>332</v>
+        <v>423</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11391,7 +11388,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11435,7 +11432,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11473,7 +11470,7 @@
       </c>
       <c r="C139" s="10"/>
       <c r="D139" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E139" s="10" t="s">
         <v>238</v>
@@ -11484,7 +11481,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>338</v>
+        <v>381</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11511,7 +11508,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>337</v>
+        <v>292</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11555,7 +11552,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>342</v>
+        <v>295</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11593,7 +11590,7 @@
       </c>
       <c r="C142" s="10"/>
       <c r="D142" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E142" s="10" t="s">
         <v>238</v>
@@ -11604,7 +11601,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>344</v>
+        <v>382</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11631,7 +11628,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>343</v>
+        <v>296</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11675,7 +11672,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11713,7 +11710,7 @@
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E145" s="10" t="s">
         <v>238</v>
@@ -11724,7 +11721,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11751,7 +11748,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -11795,7 +11792,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>348</v>
+        <v>299</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -11833,7 +11830,7 @@
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E148" s="10" t="s">
         <v>238</v>
@@ -11844,7 +11841,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>350</v>
+        <v>379</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11871,7 +11868,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>349</v>
+        <v>300</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -11915,7 +11912,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>503</v>
+        <v>351</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -11953,7 +11950,7 @@
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E151" s="10" t="s">
         <v>238</v>
@@ -11964,7 +11961,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>505</v>
+        <v>408</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -11991,7 +11988,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>504</v>
+        <v>352</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -12035,7 +12032,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>351</v>
+        <v>301</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -12073,7 +12070,7 @@
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E154" s="10" t="s">
         <v>238</v>
@@ -12084,7 +12081,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>353</v>
+        <v>422</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12111,7 +12108,7 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12155,7 +12152,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>449</v>
+        <v>533</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12193,7 +12190,7 @@
       </c>
       <c r="C157" s="10"/>
       <c r="D157" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E157" s="10" t="s">
         <v>238</v>
@@ -12204,7 +12201,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>454</v>
+        <v>411</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12231,7 +12228,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12275,7 +12272,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>464</v>
+        <v>534</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12313,7 +12310,7 @@
       </c>
       <c r="C160" s="10"/>
       <c r="D160" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>238</v>
@@ -12324,7 +12321,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>466</v>
+        <v>412</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12351,7 +12348,7 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>465</v>
+        <v>535</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12395,7 +12392,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>467</v>
+        <v>536</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>235</v>
@@ -12433,7 +12430,7 @@
       </c>
       <c r="C163" s="10"/>
       <c r="D163" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E163" s="10" t="s">
         <v>238</v>
@@ -12444,7 +12441,7 @@
       </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10" t="s">
-        <v>469</v>
+        <v>413</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="10"/>
@@ -12471,7 +12468,7 @@
       </c>
       <c r="C164" s="41"/>
       <c r="D164" s="41" t="s">
-        <v>468</v>
+        <v>537</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>237</v>
@@ -12515,7 +12512,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>451</v>
+        <v>538</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>235</v>
@@ -12553,7 +12550,7 @@
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E166" s="10" t="s">
         <v>238</v>
@@ -12564,7 +12561,7 @@
       </c>
       <c r="H166" s="10"/>
       <c r="I166" s="10" t="s">
-        <v>453</v>
+        <v>414</v>
       </c>
       <c r="J166" s="10"/>
       <c r="K166" s="10"/>
@@ -12591,7 +12588,7 @@
       </c>
       <c r="C167" s="41"/>
       <c r="D167" s="41" t="s">
-        <v>452</v>
+        <v>539</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>237</v>
@@ -12635,7 +12632,7 @@
         <v>1</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>455</v>
+        <v>540</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>235</v>
@@ -12673,7 +12670,7 @@
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E169" s="10" t="s">
         <v>238</v>
@@ -12684,7 +12681,7 @@
       </c>
       <c r="H169" s="10"/>
       <c r="I169" s="10" t="s">
-        <v>457</v>
+        <v>415</v>
       </c>
       <c r="J169" s="10"/>
       <c r="K169" s="10"/>
@@ -12711,7 +12708,7 @@
       </c>
       <c r="C170" s="41"/>
       <c r="D170" s="41" t="s">
-        <v>456</v>
+        <v>541</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>237</v>
@@ -12755,7 +12752,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>477</v>
+        <v>542</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>235</v>
@@ -12793,7 +12790,7 @@
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E172" s="10" t="s">
         <v>238</v>
@@ -12804,7 +12801,7 @@
       </c>
       <c r="H172" s="10"/>
       <c r="I172" s="10" t="s">
-        <v>479</v>
+        <v>416</v>
       </c>
       <c r="J172" s="10"/>
       <c r="K172" s="10"/>
@@ -12831,7 +12828,7 @@
       </c>
       <c r="C173" s="41"/>
       <c r="D173" s="41" t="s">
-        <v>478</v>
+        <v>543</v>
       </c>
       <c r="E173" s="41" t="s">
         <v>237</v>
@@ -12875,7 +12872,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>458</v>
+        <v>544</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>235</v>
@@ -12913,7 +12910,7 @@
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E175" s="10" t="s">
         <v>238</v>
@@ -12924,7 +12921,7 @@
       </c>
       <c r="H175" s="10"/>
       <c r="I175" s="10" t="s">
-        <v>460</v>
+        <v>417</v>
       </c>
       <c r="J175" s="10"/>
       <c r="K175" s="10"/>
@@ -12951,7 +12948,7 @@
       </c>
       <c r="C176" s="41"/>
       <c r="D176" s="41" t="s">
-        <v>459</v>
+        <v>545</v>
       </c>
       <c r="E176" s="41" t="s">
         <v>237</v>
@@ -12995,7 +12992,7 @@
         <v>1</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>461</v>
+        <v>546</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>235</v>
@@ -13033,7 +13030,7 @@
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E178" s="10" t="s">
         <v>238</v>
@@ -13044,7 +13041,7 @@
       </c>
       <c r="H178" s="10"/>
       <c r="I178" s="10" t="s">
-        <v>463</v>
+        <v>418</v>
       </c>
       <c r="J178" s="10"/>
       <c r="K178" s="10"/>
@@ -13071,7 +13068,7 @@
       </c>
       <c r="C179" s="41"/>
       <c r="D179" s="41" t="s">
-        <v>462</v>
+        <v>547</v>
       </c>
       <c r="E179" s="41" t="s">
         <v>237</v>
@@ -13115,16 +13112,16 @@
         <v>1</v>
       </c>
       <c r="B180" s="42" t="s">
-        <v>327</v>
+        <v>284</v>
       </c>
       <c r="C180" s="42" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="D180" s="42" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="E180" s="42" t="s">
-        <v>326</v>
+        <v>283</v>
       </c>
       <c r="F180" s="42"/>
       <c r="G180" s="42"/>
@@ -13151,16 +13148,16 @@
         <v>1</v>
       </c>
       <c r="B181" s="42" t="s">
-        <v>513</v>
+        <v>356</v>
       </c>
       <c r="C181" s="42" t="s">
-        <v>512</v>
+        <v>355</v>
       </c>
       <c r="D181" s="42" t="s">
-        <v>512</v>
+        <v>355</v>
       </c>
       <c r="E181" s="42" t="s">
-        <v>326</v>
+        <v>283</v>
       </c>
       <c r="F181" s="42"/>
       <c r="G181" s="42"/>
@@ -13202,8 +13199,8 @@
   <dimension ref="A1:M81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13319,16 +13316,16 @@
     </row>
     <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>357</v>
+        <v>305</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>399</v>
+        <v>437</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G4" s="15" t="b">
         <v>0</v>
@@ -13346,16 +13343,16 @@
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>358</v>
+        <v>306</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>400</v>
+        <v>468</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G5" s="15" t="b">
         <v>0</v>
@@ -13373,16 +13370,16 @@
     </row>
     <row r="6" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>359</v>
+        <v>307</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>360</v>
+        <v>489</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G6" s="15" t="b">
         <v>0</v>
@@ -13400,16 +13397,16 @@
     </row>
     <row r="7" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>361</v>
+        <v>308</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>401</v>
+        <v>452</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G7" s="15" t="b">
         <v>0</v>
@@ -13427,16 +13424,16 @@
     </row>
     <row r="8" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>362</v>
+        <v>309</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>402</v>
+        <v>488</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G8" s="15" t="b">
         <v>0</v>
@@ -13454,16 +13451,16 @@
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>363</v>
+        <v>494</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>403</v>
+        <v>447</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G9" s="15" t="b">
         <v>0</v>
@@ -13481,16 +13478,16 @@
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>364</v>
+        <v>495</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>404</v>
+        <v>449</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G10" s="15" t="b">
         <v>0</v>
@@ -13508,16 +13505,16 @@
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>365</v>
+        <v>496</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>405</v>
+        <v>450</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G11" s="15" t="b">
         <v>0</v>
@@ -13535,16 +13532,16 @@
     </row>
     <row r="12" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>366</v>
+        <v>497</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>406</v>
+        <v>448</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G12" s="15" t="b">
         <v>0</v>
@@ -13562,16 +13559,16 @@
     </row>
     <row r="13" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>367</v>
+        <v>310</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>368</v>
+        <v>451</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G13" s="15" t="b">
         <v>0</v>
@@ -13589,16 +13586,16 @@
     </row>
     <row r="14" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>369</v>
+        <v>311</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>370</v>
+        <v>478</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G14" s="15" t="b">
         <v>0</v>
@@ -13616,16 +13613,16 @@
     </row>
     <row r="15" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>437</v>
+        <v>334</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G15" s="15" t="b">
         <v>0</v>
@@ -13643,16 +13640,16 @@
     </row>
     <row r="16" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>442</v>
+        <v>337</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>443</v>
+        <v>479</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G16" s="15" t="b">
         <v>0</v>
@@ -13669,15 +13666,15 @@
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>387</v>
+      <c r="A17" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="B17" s="21"/>
       <c r="D17" s="15" t="s">
-        <v>423</v>
+        <v>442</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G17" s="15" t="b">
         <v>0</v>
@@ -13690,15 +13687,15 @@
       </c>
     </row>
     <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>489</v>
+      <c r="A18" s="15" t="s">
+        <v>341</v>
       </c>
       <c r="B18" s="21"/>
       <c r="D18" s="15" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G18" s="15" t="b">
         <v>0</v>
@@ -13712,16 +13709,16 @@
     </row>
     <row r="19" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>432</v>
+        <v>331</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>433</v>
+        <v>477</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G19" s="15" t="b">
         <v>0</v>
@@ -13739,16 +13736,16 @@
     </row>
     <row r="20" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>371</v>
+        <v>312</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>407</v>
+        <v>464</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G20" s="15" t="b">
         <v>0</v>
@@ -13766,16 +13763,16 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>372</v>
+        <v>498</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>408</v>
+        <v>466</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G21" s="15" t="b">
         <v>0</v>
@@ -13793,16 +13790,16 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>373</v>
+        <v>499</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>409</v>
+        <v>462</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G22" s="15" t="b">
         <v>0</v>
@@ -13820,16 +13817,16 @@
     </row>
     <row r="23" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>374</v>
+        <v>313</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>410</v>
+        <v>463</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G23" s="15" t="b">
         <v>0</v>
@@ -13846,15 +13843,15 @@
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
-        <v>375</v>
+      <c r="A24" s="15" t="s">
+        <v>500</v>
       </c>
       <c r="B24" s="21"/>
       <c r="D24" s="15" t="s">
-        <v>411</v>
+        <v>459</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G24" s="15" t="b">
         <v>0</v>
@@ -13867,15 +13864,15 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
-        <v>376</v>
+      <c r="A25" s="15" t="s">
+        <v>314</v>
       </c>
       <c r="B25" s="21"/>
       <c r="D25" s="15" t="s">
-        <v>412</v>
+        <v>465</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G25" s="15" t="b">
         <v>0</v>
@@ -13888,15 +13885,15 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
-        <v>377</v>
+      <c r="A26" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="15" t="s">
-        <v>413</v>
+        <v>460</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G26" s="15" t="b">
         <v>0</v>
@@ -13909,15 +13906,15 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
-        <v>378</v>
+      <c r="A27" s="15" t="s">
+        <v>501</v>
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="15" t="s">
-        <v>414</v>
+        <v>461</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G27" s="15" t="b">
         <v>0</v>
@@ -13930,15 +13927,15 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
-        <v>447</v>
+      <c r="A28" s="15" t="s">
+        <v>340</v>
       </c>
       <c r="B28" s="21"/>
       <c r="D28" s="15" t="s">
-        <v>448</v>
+        <v>487</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G28" s="15" t="b">
         <v>0</v>
@@ -13951,15 +13948,15 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
-        <v>379</v>
+      <c r="A29" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="B29" s="21"/>
       <c r="D29" s="15" t="s">
-        <v>415</v>
+        <v>490</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G29" s="15" t="b">
         <v>0</v>
@@ -13972,15 +13969,15 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
-        <v>380</v>
+      <c r="A30" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="B30" s="21"/>
       <c r="D30" s="15" t="s">
-        <v>416</v>
+        <v>445</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G30" s="15" t="b">
         <v>0</v>
@@ -13993,15 +13990,15 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
-        <v>381</v>
+      <c r="A31" s="15" t="s">
+        <v>318</v>
       </c>
       <c r="B31" s="21"/>
       <c r="D31" s="15" t="s">
-        <v>417</v>
+        <v>482</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G31" s="15" t="b">
         <v>0</v>
@@ -14014,15 +14011,15 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
-        <v>382</v>
+      <c r="A32" s="15" t="s">
+        <v>319</v>
       </c>
       <c r="B32" s="21"/>
       <c r="D32" s="15" t="s">
-        <v>418</v>
+        <v>446</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G32" s="15" t="b">
         <v>0</v>
@@ -14035,15 +14032,15 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
-        <v>383</v>
+      <c r="A33" s="15" t="s">
+        <v>502</v>
       </c>
       <c r="B33" s="21"/>
       <c r="D33" s="15" t="s">
-        <v>419</v>
+        <v>485</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G33" s="15" t="b">
         <v>0</v>
@@ -14056,15 +14053,15 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="s">
-        <v>384</v>
+      <c r="A34" s="15" t="s">
+        <v>503</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="15" t="s">
-        <v>420</v>
+        <v>484</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G34" s="15" t="b">
         <v>0</v>
@@ -14077,15 +14074,15 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
-        <v>385</v>
+      <c r="A35" s="15" t="s">
+        <v>504</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="15" t="s">
-        <v>421</v>
+        <v>486</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G35" s="15" t="b">
         <v>0</v>
@@ -14098,15 +14095,15 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
-        <v>386</v>
+      <c r="A36" s="15" t="s">
+        <v>505</v>
       </c>
       <c r="B36" s="21"/>
       <c r="D36" s="15" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G36" s="15" t="b">
         <v>0</v>
@@ -14119,15 +14116,15 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="44" t="s">
-        <v>388</v>
+      <c r="A37" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="B37" s="21"/>
       <c r="D37" s="15" t="s">
-        <v>396</v>
+        <v>443</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G37" s="15" t="b">
         <v>0</v>
@@ -14140,15 +14137,15 @@
       </c>
     </row>
     <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="s">
-        <v>497</v>
+      <c r="A38" s="15" t="s">
+        <v>346</v>
       </c>
       <c r="B38" s="21"/>
       <c r="D38" s="15" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G38" s="15" t="b">
         <v>0</v>
@@ -14161,15 +14158,15 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
-        <v>389</v>
+      <c r="A39" s="15" t="s">
+        <v>322</v>
       </c>
       <c r="B39" s="21"/>
       <c r="D39" s="15" t="s">
-        <v>424</v>
+        <v>491</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G39" s="15" t="b">
         <v>0</v>
@@ -14182,15 +14179,15 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
-        <v>543</v>
+      <c r="A40" s="15" t="s">
+        <v>376</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>544</v>
+        <v>453</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G40" s="15" t="b">
         <v>0</v>
@@ -14203,15 +14200,15 @@
       </c>
     </row>
     <row r="41" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
-        <v>541</v>
+      <c r="A41" s="15" t="s">
+        <v>375</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>542</v>
+        <v>454</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G41" s="15" t="b">
         <v>0</v>
@@ -14224,15 +14221,15 @@
       </c>
     </row>
     <row r="42" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
-        <v>524</v>
+      <c r="A42" s="15" t="s">
+        <v>365</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>525</v>
+        <v>458</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G42" s="15" t="b">
         <v>0</v>
@@ -14245,15 +14242,15 @@
       </c>
     </row>
     <row r="43" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
-        <v>526</v>
+      <c r="A43" s="15" t="s">
+        <v>366</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>537</v>
+        <v>455</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G43" s="15" t="b">
         <v>0</v>
@@ -14266,15 +14263,15 @@
       </c>
     </row>
     <row r="44" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
-        <v>528</v>
+      <c r="A44" s="15" t="s">
+        <v>368</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>536</v>
+        <v>457</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G44" s="15" t="b">
         <v>0</v>
@@ -14287,15 +14284,15 @@
       </c>
     </row>
     <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
-        <v>527</v>
+      <c r="A45" s="15" t="s">
+        <v>367</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>535</v>
+        <v>456</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G45" s="15" t="b">
         <v>0</v>
@@ -14308,15 +14305,15 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
-        <v>390</v>
+      <c r="A46" s="15" t="s">
+        <v>323</v>
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>397</v>
+        <v>481</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G46" s="15" t="b">
         <v>0</v>
@@ -14329,15 +14326,15 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>391</v>
+      <c r="A47" s="15" t="s">
+        <v>324</v>
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G47" s="15" t="b">
         <v>0</v>
@@ -14350,15 +14347,15 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
-        <v>392</v>
+      <c r="A48" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>398</v>
+        <v>441</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G48" s="15" t="b">
         <v>0</v>
@@ -14371,15 +14368,15 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
-        <v>393</v>
+      <c r="A49" s="15" t="s">
+        <v>326</v>
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G49" s="15" t="b">
         <v>0</v>
@@ -14392,15 +14389,15 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="44" t="s">
-        <v>394</v>
+      <c r="A50" s="15" t="s">
+        <v>327</v>
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G50" s="15" t="b">
         <v>0</v>
@@ -14413,15 +14410,15 @@
       </c>
     </row>
     <row r="51" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="44" t="s">
-        <v>506</v>
+      <c r="A51" s="15" t="s">
+        <v>353</v>
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>507</v>
+        <v>467</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G51" s="15" t="b">
         <v>0</v>
@@ -14434,15 +14431,15 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="44" t="s">
-        <v>395</v>
+      <c r="A52" s="15" t="s">
+        <v>328</v>
       </c>
       <c r="B52" s="21"/>
       <c r="D52" s="15" t="s">
-        <v>428</v>
+        <v>480</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G52" s="15" t="b">
         <v>0</v>
@@ -14455,16 +14452,16 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
-        <v>470</v>
+      <c r="A53" s="15" t="s">
+        <v>506</v>
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="15" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G53" s="15" t="b">
         <v>0</v>
@@ -14477,16 +14474,16 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="s">
-        <v>471</v>
+      <c r="A54" s="15" t="s">
+        <v>507</v>
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="15" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G54" s="15" t="b">
         <v>0</v>
@@ -14499,16 +14496,16 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="44" t="s">
-        <v>472</v>
+      <c r="A55" s="15" t="s">
+        <v>508</v>
       </c>
       <c r="B55" s="21"/>
       <c r="D55" s="15" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G55" s="15" t="b">
         <v>0</v>
@@ -14521,16 +14518,16 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="s">
-        <v>473</v>
+      <c r="A56" s="15" t="s">
+        <v>509</v>
       </c>
       <c r="B56" s="21"/>
       <c r="D56" s="15" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="E56" s="22"/>
       <c r="F56" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G56" s="15" t="b">
         <v>0</v>
@@ -14543,16 +14540,16 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="44" t="s">
-        <v>474</v>
+      <c r="A57" s="15" t="s">
+        <v>510</v>
       </c>
       <c r="B57" s="21"/>
       <c r="D57" s="15" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G57" s="15" t="b">
         <v>0</v>
@@ -14565,16 +14562,16 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="44" t="s">
-        <v>476</v>
+      <c r="A58" s="15" t="s">
+        <v>511</v>
       </c>
       <c r="B58" s="21"/>
       <c r="D58" s="15" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
       <c r="E58" s="22"/>
       <c r="F58" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G58" s="15" t="b">
         <v>0</v>
@@ -14587,16 +14584,16 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="44" t="s">
-        <v>475</v>
+      <c r="A59" s="15" t="s">
+        <v>512</v>
       </c>
       <c r="B59" s="21"/>
       <c r="D59" s="15" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G59" s="15" t="b">
         <v>0</v>
@@ -14609,16 +14606,16 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="44" t="s">
-        <v>480</v>
+      <c r="A60" s="15" t="s">
+        <v>513</v>
       </c>
       <c r="B60" s="21"/>
       <c r="D60" s="15" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="15" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G60" s="15" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update to OS 1.11.5; revert 1-spd ASHP workaround.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -1098,9 +1098,6 @@
     <t>Lighting</t>
   </si>
   <si>
-    <t>1.15.7-resstock</t>
-  </si>
-  <si>
     <t>ServerDirectoryCleanup</t>
   </si>
   <si>
@@ -1678,6 +1675,9 @@
   </si>
   <si>
     <t>Misc Well Pump Sample Value</t>
+  </si>
+  <si>
+    <t>1.18.0-rc0</t>
   </si>
 </sst>
 </file>
@@ -1713,6 +1713,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1720,6 +1721,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1741,6 +1743,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5257,9 +5260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5318,7 +5319,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>354</v>
+        <v>547</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
@@ -5386,7 +5387,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5394,7 +5395,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$6.72/hour</v>
+        <v>$1.68/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>202</v>
@@ -5549,14 +5550,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="E24" s="22"/>
     </row>
@@ -5764,7 +5765,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5820,13 +5821,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
+        <v>356</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="C44" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -6201,7 +6202,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6321,7 +6322,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6441,7 +6442,7 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -6561,7 +6562,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6681,7 +6682,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6801,7 +6802,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -6921,7 +6922,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7041,7 +7042,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -7161,7 +7162,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7281,7 +7282,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7401,7 +7402,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7521,7 +7522,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7641,7 +7642,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7761,7 +7762,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -7881,7 +7882,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -8001,7 +8002,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -8121,7 +8122,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8192,7 +8193,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>235</v>
@@ -8241,7 +8242,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8268,7 +8269,7 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E59" s="41" t="s">
         <v>237</v>
@@ -8312,7 +8313,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>235</v>
@@ -8361,7 +8362,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8388,7 +8389,7 @@
       </c>
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>237</v>
@@ -8481,7 +8482,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8552,7 +8553,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>235</v>
@@ -8601,7 +8602,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8628,7 +8629,7 @@
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="41" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>237</v>
@@ -8721,7 +8722,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8841,7 +8842,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -8912,7 +8913,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C75" s="40" t="s">
         <v>235</v>
@@ -8961,7 +8962,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -8988,7 +8989,7 @@
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>237</v>
@@ -9032,7 +9033,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C78" s="40" t="s">
         <v>235</v>
@@ -9081,7 +9082,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -9108,7 +9109,7 @@
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>237</v>
@@ -9201,7 +9202,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9321,7 +9322,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9441,7 +9442,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9561,7 +9562,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9681,7 +9682,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9752,7 +9753,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>235</v>
@@ -9801,7 +9802,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9828,7 +9829,7 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>237</v>
@@ -9872,7 +9873,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>235</v>
@@ -9921,7 +9922,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9948,7 +9949,7 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>237</v>
@@ -9992,7 +9993,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>235</v>
@@ -10041,7 +10042,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -10068,7 +10069,7 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>237</v>
@@ -10112,7 +10113,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>235</v>
@@ -10161,7 +10162,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10188,7 +10189,7 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>237</v>
@@ -10281,7 +10282,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10401,7 +10402,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10521,7 +10522,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10592,7 +10593,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10641,7 +10642,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10668,7 +10669,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10712,7 +10713,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10761,7 +10762,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10788,7 +10789,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10832,7 +10833,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -10881,7 +10882,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -10908,7 +10909,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -10952,7 +10953,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -11001,7 +11002,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -11028,7 +11029,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -11072,7 +11073,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11121,7 +11122,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11148,7 +11149,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11192,7 +11193,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11241,7 +11242,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11268,7 +11269,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11361,7 +11362,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11481,7 +11482,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11601,7 +11602,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11721,7 +11722,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11841,7 +11842,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11961,7 +11962,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -12081,7 +12082,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12152,7 +12153,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12201,7 +12202,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12228,7 +12229,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12272,7 +12273,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12321,7 +12322,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12348,7 +12349,7 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12392,7 +12393,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>235</v>
@@ -12441,7 +12442,7 @@
       </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="10"/>
@@ -12468,7 +12469,7 @@
       </c>
       <c r="C164" s="41"/>
       <c r="D164" s="41" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>237</v>
@@ -12512,7 +12513,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>235</v>
@@ -12561,7 +12562,7 @@
       </c>
       <c r="H166" s="10"/>
       <c r="I166" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J166" s="10"/>
       <c r="K166" s="10"/>
@@ -12588,7 +12589,7 @@
       </c>
       <c r="C167" s="41"/>
       <c r="D167" s="41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>237</v>
@@ -12632,7 +12633,7 @@
         <v>1</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>235</v>
@@ -12681,7 +12682,7 @@
       </c>
       <c r="H169" s="10"/>
       <c r="I169" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J169" s="10"/>
       <c r="K169" s="10"/>
@@ -12708,7 +12709,7 @@
       </c>
       <c r="C170" s="41"/>
       <c r="D170" s="41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>237</v>
@@ -12752,7 +12753,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>235</v>
@@ -12801,7 +12802,7 @@
       </c>
       <c r="H172" s="10"/>
       <c r="I172" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J172" s="10"/>
       <c r="K172" s="10"/>
@@ -12828,7 +12829,7 @@
       </c>
       <c r="C173" s="41"/>
       <c r="D173" s="41" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E173" s="41" t="s">
         <v>237</v>
@@ -12872,7 +12873,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>235</v>
@@ -12921,7 +12922,7 @@
       </c>
       <c r="H175" s="10"/>
       <c r="I175" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J175" s="10"/>
       <c r="K175" s="10"/>
@@ -12948,7 +12949,7 @@
       </c>
       <c r="C176" s="41"/>
       <c r="D176" s="41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E176" s="41" t="s">
         <v>237</v>
@@ -12992,7 +12993,7 @@
         <v>1</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>235</v>
@@ -13041,7 +13042,7 @@
       </c>
       <c r="H178" s="10"/>
       <c r="I178" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J178" s="10"/>
       <c r="K178" s="10"/>
@@ -13068,7 +13069,7 @@
       </c>
       <c r="C179" s="41"/>
       <c r="D179" s="41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E179" s="41" t="s">
         <v>237</v>
@@ -13148,13 +13149,13 @@
         <v>1</v>
       </c>
       <c r="B181" s="42" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C181" s="42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D181" s="42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E181" s="42" t="s">
         <v>283</v>
@@ -13321,7 +13322,7 @@
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15" t="s">
@@ -13348,7 +13349,7 @@
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15" t="s">
@@ -13375,7 +13376,7 @@
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15" t="s">
@@ -13402,7 +13403,7 @@
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
@@ -13429,7 +13430,7 @@
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15" t="s">
@@ -13451,12 +13452,12 @@
     </row>
     <row r="9" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15" t="s">
@@ -13478,12 +13479,12 @@
     </row>
     <row r="10" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
@@ -13505,12 +13506,12 @@
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
@@ -13532,12 +13533,12 @@
     </row>
     <row r="12" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15" t="s">
@@ -13564,7 +13565,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15" t="s">
@@ -13591,7 +13592,7 @@
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15" t="s">
@@ -13618,7 +13619,7 @@
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
@@ -13645,7 +13646,7 @@
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
@@ -13671,7 +13672,7 @@
       </c>
       <c r="B17" s="21"/>
       <c r="D17" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>286</v>
@@ -13692,7 +13693,7 @@
       </c>
       <c r="B18" s="21"/>
       <c r="D18" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>286</v>
@@ -13714,7 +13715,7 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15" t="s">
@@ -13741,7 +13742,7 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15" t="s">
@@ -13763,12 +13764,12 @@
     </row>
     <row r="21" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
@@ -13790,12 +13791,12 @@
     </row>
     <row r="22" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15" t="s">
@@ -13822,7 +13823,7 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
@@ -13844,11 +13845,11 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B24" s="21"/>
       <c r="D24" s="15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>286</v>
@@ -13869,7 +13870,7 @@
       </c>
       <c r="B25" s="21"/>
       <c r="D25" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>286</v>
@@ -13890,7 +13891,7 @@
       </c>
       <c r="B26" s="21"/>
       <c r="D26" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>286</v>
@@ -13907,11 +13908,11 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B27" s="21"/>
       <c r="D27" s="15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>286</v>
@@ -13932,7 +13933,7 @@
       </c>
       <c r="B28" s="21"/>
       <c r="D28" s="15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>286</v>
@@ -13953,7 +13954,7 @@
       </c>
       <c r="B29" s="21"/>
       <c r="D29" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>286</v>
@@ -13974,7 +13975,7 @@
       </c>
       <c r="B30" s="21"/>
       <c r="D30" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>286</v>
@@ -13995,7 +13996,7 @@
       </c>
       <c r="B31" s="21"/>
       <c r="D31" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>286</v>
@@ -14016,7 +14017,7 @@
       </c>
       <c r="B32" s="21"/>
       <c r="D32" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>286</v>
@@ -14033,11 +14034,11 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B33" s="21"/>
       <c r="D33" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>286</v>
@@ -14054,11 +14055,11 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B34" s="21"/>
       <c r="D34" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>286</v>
@@ -14075,11 +14076,11 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B35" s="21"/>
       <c r="D35" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>286</v>
@@ -14096,11 +14097,11 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B36" s="21"/>
       <c r="D36" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>286</v>
@@ -14121,7 +14122,7 @@
       </c>
       <c r="B37" s="21"/>
       <c r="D37" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>286</v>
@@ -14142,7 +14143,7 @@
       </c>
       <c r="B38" s="21"/>
       <c r="D38" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>286</v>
@@ -14163,7 +14164,7 @@
       </c>
       <c r="B39" s="21"/>
       <c r="D39" s="15" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>286</v>
@@ -14180,11 +14181,11 @@
     </row>
     <row r="40" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B40" s="21"/>
       <c r="D40" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>286</v>
@@ -14201,11 +14202,11 @@
     </row>
     <row r="41" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B41" s="21"/>
       <c r="D41" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>286</v>
@@ -14222,11 +14223,11 @@
     </row>
     <row r="42" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B42" s="21"/>
       <c r="D42" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>286</v>
@@ -14243,11 +14244,11 @@
     </row>
     <row r="43" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B43" s="21"/>
       <c r="D43" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>286</v>
@@ -14264,11 +14265,11 @@
     </row>
     <row r="44" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B44" s="21"/>
       <c r="D44" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>286</v>
@@ -14285,11 +14286,11 @@
     </row>
     <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B45" s="21"/>
       <c r="D45" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>286</v>
@@ -14310,7 +14311,7 @@
       </c>
       <c r="B46" s="21"/>
       <c r="D46" s="15" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>286</v>
@@ -14331,7 +14332,7 @@
       </c>
       <c r="B47" s="21"/>
       <c r="D47" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>286</v>
@@ -14352,7 +14353,7 @@
       </c>
       <c r="B48" s="21"/>
       <c r="D48" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>286</v>
@@ -14373,7 +14374,7 @@
       </c>
       <c r="B49" s="21"/>
       <c r="D49" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F49" s="15" t="s">
         <v>286</v>
@@ -14394,7 +14395,7 @@
       </c>
       <c r="B50" s="21"/>
       <c r="D50" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F50" s="15" t="s">
         <v>286</v>
@@ -14415,7 +14416,7 @@
       </c>
       <c r="B51" s="21"/>
       <c r="D51" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F51" s="15" t="s">
         <v>286</v>
@@ -14436,7 +14437,7 @@
       </c>
       <c r="B52" s="21"/>
       <c r="D52" s="15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F52" s="15" t="s">
         <v>286</v>
@@ -14453,11 +14454,11 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B53" s="21"/>
       <c r="D53" s="15" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="15" t="s">
@@ -14475,11 +14476,11 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B54" s="21"/>
       <c r="D54" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="15" t="s">
@@ -14497,11 +14498,11 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B55" s="21"/>
       <c r="D55" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E55" s="22"/>
       <c r="F55" s="15" t="s">
@@ -14519,11 +14520,11 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B56" s="21"/>
       <c r="D56" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E56" s="22"/>
       <c r="F56" s="15" t="s">
@@ -14541,11 +14542,11 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B57" s="21"/>
       <c r="D57" s="15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="15" t="s">
@@ -14563,11 +14564,11 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B58" s="21"/>
       <c r="D58" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E58" s="22"/>
       <c r="F58" s="15" t="s">
@@ -14585,11 +14586,11 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B59" s="21"/>
       <c r="D59" s="15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="15" t="s">
@@ -14607,11 +14608,11 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B60" s="21"/>
       <c r="D60" s="15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="15" t="s">

</xml_diff>

<commit_message>
The results csv for upgrades now reference the existing building datapoint name. Also simplified how we generate outputs for the results csv.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -5260,7 +5260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5550,14 +5552,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="E24" s="22"/>
     </row>
@@ -13201,7 +13203,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added simulation outputs (total, by end use, by fuel type) to the results CSV files.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8295" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="8295" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -29,12 +29,12 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="586">
   <si>
     <t>type</t>
   </si>
@@ -1678,6 +1678,120 @@
   </si>
   <si>
     <t>1.18.0-rc0</t>
+  </si>
+  <si>
+    <t>Standard Reports</t>
+  </si>
+  <si>
+    <t>StandardReports</t>
+  </si>
+  <si>
+    <t>Total Site Energy MBtu</t>
+  </si>
+  <si>
+    <t>Total Site Electricity kWh</t>
+  </si>
+  <si>
+    <t>Total Site Natural Gas therm</t>
+  </si>
+  <si>
+    <t>Total Site Other Fuel MBtu</t>
+  </si>
+  <si>
+    <t>Electricity Heating kWh</t>
+  </si>
+  <si>
+    <t>Electricity Cooling kWh</t>
+  </si>
+  <si>
+    <t>Electricity Interior Lighting kWh</t>
+  </si>
+  <si>
+    <t>Electricity Exterior Lighting kWh</t>
+  </si>
+  <si>
+    <t>Electricity Interior Equipment kWh</t>
+  </si>
+  <si>
+    <t>Electricity Fans kWh</t>
+  </si>
+  <si>
+    <t>Electricity Pumps kWh</t>
+  </si>
+  <si>
+    <t>Electricity Water Systems kWh</t>
+  </si>
+  <si>
+    <t>Natural Gas Heating therm</t>
+  </si>
+  <si>
+    <t>Natural Gas Interior Equipment therm</t>
+  </si>
+  <si>
+    <t>Natural Gas Water Systems therm</t>
+  </si>
+  <si>
+    <t>Other Fuel Heating MBtu</t>
+  </si>
+  <si>
+    <t>Other Fuel Interior Equipment MBtu</t>
+  </si>
+  <si>
+    <t>Other Fuel Water Systems MBtu</t>
+  </si>
+  <si>
+    <t>standard_reports.Other Fuel Water Systems MBtu</t>
+  </si>
+  <si>
+    <t>standard_reports.Other Fuel Interior Equipment MBtu</t>
+  </si>
+  <si>
+    <t>standard_reports.Other Fuel Heating MBtu</t>
+  </si>
+  <si>
+    <t>standard_reports.Natural Gas Water Systems therm</t>
+  </si>
+  <si>
+    <t>standard_reports.Natural Gas Interior Equipment therm</t>
+  </si>
+  <si>
+    <t>standard_reports.Total Site Energy MBtu</t>
+  </si>
+  <si>
+    <t>standard_reports.Total Site Electricity kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Total Site Natural Gas therm</t>
+  </si>
+  <si>
+    <t>standard_reports.Total Site Other Fuel MBtu</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Heating kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Cooling kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Interior Lighting kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Exterior Lighting kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Interior Equipment kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Fans kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Pumps kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Electricity Water Systems kWh</t>
+  </si>
+  <si>
+    <t>standard_reports.Natural Gas Heating therm</t>
   </si>
 </sst>
 </file>
@@ -1754,7 +1868,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1833,6 +1947,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3357,7 +3477,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3455,6 +3575,9 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5260,9 +5383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5897,7 +6018,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z181"/>
+  <dimension ref="A1:Z182"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -13151,13 +13272,13 @@
         <v>1</v>
       </c>
       <c r="B181" s="42" t="s">
-        <v>355</v>
+        <v>548</v>
       </c>
       <c r="C181" s="42" t="s">
-        <v>354</v>
+        <v>549</v>
       </c>
       <c r="D181" s="42" t="s">
-        <v>354</v>
+        <v>549</v>
       </c>
       <c r="E181" s="42" t="s">
         <v>283</v>
@@ -13182,6 +13303,42 @@
       <c r="W181" s="42"/>
       <c r="X181" s="42"/>
     </row>
+    <row r="182" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A182" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B182" s="42" t="s">
+        <v>355</v>
+      </c>
+      <c r="C182" s="42" t="s">
+        <v>354</v>
+      </c>
+      <c r="D182" s="42" t="s">
+        <v>354</v>
+      </c>
+      <c r="E182" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="F182" s="42"/>
+      <c r="G182" s="42"/>
+      <c r="H182" s="43"/>
+      <c r="I182" s="43"/>
+      <c r="J182" s="42"/>
+      <c r="K182" s="42"/>
+      <c r="L182" s="42"/>
+      <c r="M182" s="42"/>
+      <c r="N182" s="42"/>
+      <c r="O182" s="42"/>
+      <c r="P182" s="42"/>
+      <c r="Q182" s="42"/>
+      <c r="R182" s="42"/>
+      <c r="S182" s="42"/>
+      <c r="T182" s="42"/>
+      <c r="U182" s="42"/>
+      <c r="V182" s="42"/>
+      <c r="W182" s="42"/>
+      <c r="X182" s="42"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
   <mergeCells count="1">
@@ -13199,16 +13356,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -13317,1381 +13474,1631 @@
       </c>
       <c r="M3" s="32"/>
     </row>
-    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
         <v>305</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50" t="s">
         <v>436</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-    </row>
-    <row r="5" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="G4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+    </row>
+    <row r="5" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50" t="s">
         <v>467</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-    </row>
-    <row r="6" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="G5" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+    </row>
+    <row r="6" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50" t="s">
         <v>488</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-    </row>
-    <row r="7" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="G6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+    </row>
+    <row r="7" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
         <v>308</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15" t="s">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50" t="s">
         <v>451</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="50"/>
+      <c r="F7" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-    </row>
-    <row r="8" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="G7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+    </row>
+    <row r="8" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50" t="s">
         <v>487</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="50"/>
+      <c r="F8" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-    </row>
-    <row r="9" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="G8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+    </row>
+    <row r="9" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
         <v>493</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50" t="s">
         <v>446</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15" t="s">
+      <c r="E9" s="50"/>
+      <c r="F9" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-    </row>
-    <row r="10" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="G9" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+    </row>
+    <row r="10" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="50" t="s">
         <v>494</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50" t="s">
         <v>448</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="E10" s="50"/>
+      <c r="F10" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="G10" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+    </row>
+    <row r="11" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="50" t="s">
         <v>495</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50" t="s">
         <v>449</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="50"/>
+      <c r="F11" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="G11" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+    </row>
+    <row r="12" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="s">
         <v>496</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50" t="s">
         <v>447</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15" t="s">
+      <c r="E12" s="50"/>
+      <c r="F12" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="G12" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+    </row>
+    <row r="13" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50" t="s">
         <v>450</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
+      <c r="E13" s="50"/>
+      <c r="F13" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="G13" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+    </row>
+    <row r="14" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15" t="s">
+      <c r="E14" s="50"/>
+      <c r="F14" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="G14" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+    </row>
+    <row r="15" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A15" s="50" t="s">
         <v>334</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50" t="s">
         <v>443</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="50"/>
+      <c r="F15" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-    </row>
-    <row r="16" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="G15" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+    </row>
+    <row r="16" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
         <v>337</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50" t="s">
         <v>478</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15" t="s">
+      <c r="E16" s="50"/>
+      <c r="F16" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="G16" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+    </row>
+    <row r="17" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
         <v>320</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="50" t="s">
         <v>441</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="G17" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="50" t="s">
         <v>341</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="50" t="s">
         <v>491</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="G18" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A19" s="50" t="s">
         <v>331</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="50"/>
+      <c r="F19" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-    </row>
-    <row r="20" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="G19" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+    </row>
+    <row r="20" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A20" s="50" t="s">
         <v>312</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50" t="s">
         <v>463</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
+      <c r="E20" s="50"/>
+      <c r="F20" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="G20" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+    </row>
+    <row r="21" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="50" t="s">
         <v>497</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50" t="s">
         <v>465</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="50"/>
+      <c r="F21" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="G21" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+    </row>
+    <row r="22" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="50" t="s">
         <v>498</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50" t="s">
         <v>461</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15" t="s">
+      <c r="E22" s="50"/>
+      <c r="F22" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" s="22" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="G22" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+    </row>
+    <row r="23" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15" t="s">
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50" t="s">
         <v>462</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15" t="s">
+      <c r="E23" s="50"/>
+      <c r="F23" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="G23" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+    </row>
+    <row r="24" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="50" t="s">
         <v>499</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="50" t="s">
         <v>458</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="G24" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="50" t="s">
         <v>314</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="50" t="s">
         <v>464</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="G25" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="50" t="s">
         <v>459</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G26" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="G26" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="50" t="s">
         <v>500</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="50" t="s">
         <v>460</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G27" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="G27" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="50" t="s">
         <v>340</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="50" t="s">
         <v>486</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G28" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="G28" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="50" t="s">
         <v>316</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="50" t="s">
         <v>489</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G29" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="G29" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
         <v>317</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="50" t="s">
         <v>444</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G30" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="G30" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
         <v>318</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="50" t="s">
         <v>481</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G31" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="G31" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="50" t="s">
         <v>445</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G32" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="G32" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="50" t="s">
         <v>501</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G33" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="G33" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="50" t="s">
         <v>502</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="50" t="s">
         <v>483</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G34" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="G34" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="s">
         <v>503</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="50" t="s">
         <v>485</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G35" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="G35" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="50" t="s">
         <v>504</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="50" t="s">
         <v>482</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G36" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="G36" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="50" t="s">
         <v>321</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="50" t="s">
         <v>442</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G37" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="G37" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="50" t="s">
         <v>346</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="50" t="s">
         <v>492</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G38" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H38" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="G38" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="50" t="s">
         <v>322</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="50" t="s">
         <v>490</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G39" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="G39" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="50" t="s">
         <v>375</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="50" t="s">
         <v>452</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G40" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="G40" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="50" t="s">
         <v>374</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="50" t="s">
         <v>453</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G41" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H41" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="G41" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="50" t="s">
         <v>364</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="50" t="s">
         <v>457</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G42" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="G42" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="50" t="s">
         <v>365</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="50" t="s">
         <v>454</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G43" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H43" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="G43" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="50" t="s">
         <v>367</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="50" t="s">
         <v>456</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G44" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I44" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="G44" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="50" t="s">
         <v>366</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="50" t="s">
         <v>455</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G45" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H45" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="G45" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="50" t="s">
         <v>323</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="50" t="s">
         <v>480</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G46" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H46" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I46" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="G46" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G47" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H47" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="G47" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="50" t="s">
         <v>440</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G48" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="G48" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="50" t="s">
         <v>438</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G49" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="G49" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G50" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="G50" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="50" t="s">
         <v>353</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="50" t="s">
         <v>466</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G51" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+      <c r="G51" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="50" t="s">
         <v>328</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="50" t="s">
         <v>479</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G52" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H52" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I52" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+      <c r="G52" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="50" t="s">
         <v>468</v>
       </c>
-      <c r="E53" s="22"/>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G53" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H53" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="G53" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="50" t="s">
         <v>469</v>
       </c>
-      <c r="E54" s="22"/>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G54" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I54" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="G54" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="50" t="s">
         <v>507</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="50" t="s">
         <v>470</v>
       </c>
-      <c r="E55" s="22"/>
-      <c r="F55" s="15" t="s">
+      <c r="F55" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G55" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="G55" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="50" t="s">
         <v>508</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="50" t="s">
         <v>471</v>
       </c>
-      <c r="E56" s="22"/>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G56" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H56" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="G56" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="50" t="s">
         <v>509</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="50" t="s">
         <v>472</v>
       </c>
-      <c r="E57" s="22"/>
-      <c r="F57" s="15" t="s">
+      <c r="F57" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G57" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="G57" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="50" t="s">
         <v>510</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="50" t="s">
         <v>473</v>
       </c>
-      <c r="E58" s="22"/>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G58" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H58" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I58" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="G58" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="50" t="s">
         <v>511</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="50" t="s">
         <v>474</v>
       </c>
-      <c r="E59" s="22"/>
-      <c r="F59" s="15" t="s">
+      <c r="F59" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G59" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H59" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="G59" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="50" t="s">
         <v>512</v>
       </c>
-      <c r="B60" s="21"/>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E60" s="22"/>
-      <c r="F60" s="15" t="s">
+      <c r="F60" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G60" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H60" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="21"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="21"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="21"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="21"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="21"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="21"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="21"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="21"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="21"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="21"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="21"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="21"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="21"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="21"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="21"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="21"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="21"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="21"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="21"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="21"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="21"/>
+      <c r="G60" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="49" t="s">
+        <v>550</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>573</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G61" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="49" t="s">
+        <v>551</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G62" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="49" t="s">
+        <v>552</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G63" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="49" t="s">
+        <v>553</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>576</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G64" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="49" t="s">
+        <v>554</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G65" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="49" t="s">
+        <v>555</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G66" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="49" t="s">
+        <v>556</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G67" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="49" t="s">
+        <v>557</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G68" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="49" t="s">
+        <v>558</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G69" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="49" t="s">
+        <v>559</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G70" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="49" t="s">
+        <v>560</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G71" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="49" t="s">
+        <v>561</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G72" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G73" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G74" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G75" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G76" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>569</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G77" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>567</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G78" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" s="14" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Latest measures and RBSA probability distributions.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -29,12 +29,12 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="591">
   <si>
     <t>type</t>
   </si>
@@ -1152,15 +1152,6 @@
     <t>HVAC System Heating Sample Value</t>
   </si>
   <si>
-    <t>Set HVAC Setpoints</t>
-  </si>
-  <si>
-    <t>HVAC Setpoints Sample Value</t>
-  </si>
-  <si>
-    <t>HVAC Setpoints</t>
-  </si>
-  <si>
     <t>Hot Water Fixtures</t>
   </si>
   <si>
@@ -1218,9 +1209,6 @@
     <t>Hot Water Fixtures.tsv</t>
   </si>
   <si>
-    <t>HVAC Setpoints.tsv</t>
-  </si>
-  <si>
     <t>HVAC System Combined.tsv</t>
   </si>
   <si>
@@ -1395,9 +1383,6 @@
     <t>res_stock_reporting.Hot Water Fixtures</t>
   </si>
   <si>
-    <t>res_stock_reporting.HVAC Setpoints</t>
-  </si>
-  <si>
     <t>res_stock_reporting.HVAC System Combined</t>
   </si>
   <si>
@@ -1792,6 +1777,36 @@
   </si>
   <si>
     <t>standard_reports.Natural Gas Heating therm</t>
+  </si>
+  <si>
+    <t>Set Cooling Setpoint</t>
+  </si>
+  <si>
+    <t>Set Heating Setpoint</t>
+  </si>
+  <si>
+    <t>Heating Setpoint Sample Value</t>
+  </si>
+  <si>
+    <t>Cooling Setpoint Sample Value</t>
+  </si>
+  <si>
+    <t>Cooling Setpoint.tsv</t>
+  </si>
+  <si>
+    <t>Heating Setpoint.tsv</t>
+  </si>
+  <si>
+    <t>Heating Setpoint</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Heating Setpoint</t>
+  </si>
+  <si>
+    <t>Cooling Setpoint</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Cooling Setpoint</t>
   </si>
 </sst>
 </file>
@@ -3572,12 +3587,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1503">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5442,7 +5457,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
@@ -6018,7 +6033,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z182"/>
+  <dimension ref="A1:Z185"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -6074,14 +6089,14 @@
       <c r="R1" s="30"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -6325,7 +6340,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6445,7 +6460,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6565,7 +6580,7 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -6685,7 +6700,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6805,7 +6820,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6925,7 +6940,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -7045,7 +7060,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7165,7 +7180,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -7285,7 +7300,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7405,7 +7420,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7525,7 +7540,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7645,7 +7660,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7765,7 +7780,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7885,7 +7900,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -8005,7 +8020,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -8125,7 +8140,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -8245,7 +8260,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8316,7 +8331,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>235</v>
@@ -8365,7 +8380,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8392,7 +8407,7 @@
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E59" s="41" t="s">
         <v>237</v>
@@ -8436,7 +8451,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>235</v>
@@ -8485,7 +8500,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8512,7 +8527,7 @@
       </c>
       <c r="C62" s="41"/>
       <c r="D62" s="41" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>237</v>
@@ -8605,7 +8620,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8676,7 +8691,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>235</v>
@@ -8725,7 +8740,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8752,7 +8767,7 @@
       </c>
       <c r="C68" s="41"/>
       <c r="D68" s="41" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>237</v>
@@ -8845,7 +8860,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -8965,7 +8980,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -9036,7 +9051,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="C75" s="40" t="s">
         <v>235</v>
@@ -9085,7 +9100,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -9112,7 +9127,7 @@
       </c>
       <c r="C77" s="41"/>
       <c r="D77" s="41" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>237</v>
@@ -9156,7 +9171,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="C78" s="40" t="s">
         <v>235</v>
@@ -9205,7 +9220,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -9232,7 +9247,7 @@
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>237</v>
@@ -9325,7 +9340,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9445,7 +9460,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9565,7 +9580,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9685,7 +9700,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9805,7 +9820,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9876,7 +9891,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>235</v>
@@ -9925,7 +9940,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9952,7 +9967,7 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>237</v>
@@ -9996,7 +10011,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>235</v>
@@ -10045,7 +10060,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -10072,7 +10087,7 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>237</v>
@@ -10116,7 +10131,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>235</v>
@@ -10165,7 +10180,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -10192,7 +10207,7 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>237</v>
@@ -10236,7 +10251,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>235</v>
@@ -10285,7 +10300,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10312,7 +10327,7 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>237</v>
@@ -10405,7 +10420,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10525,7 +10540,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10645,7 +10660,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10716,7 +10731,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10765,7 +10780,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10792,7 +10807,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10836,7 +10851,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10912,7 +10927,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10956,7 +10971,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -11005,7 +11020,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -11032,7 +11047,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -11076,7 +11091,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -11125,7 +11140,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -11152,7 +11167,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -11196,7 +11211,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11245,7 +11260,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11272,7 +11287,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11316,7 +11331,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>369</v>
+        <v>582</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11365,7 +11380,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>396</v>
+        <v>586</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11392,7 +11407,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>370</v>
+        <v>583</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11436,7 +11451,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>287</v>
+        <v>581</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11485,7 +11500,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>422</v>
+        <v>585</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11512,7 +11527,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>288</v>
+        <v>584</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11556,7 +11571,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11605,7 +11620,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>380</v>
+        <v>418</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11632,7 +11647,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11676,7 +11691,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11725,7 +11740,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11752,7 +11767,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11796,7 +11811,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11845,7 +11860,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11872,7 +11887,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -11916,7 +11931,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -11965,7 +11980,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -11992,7 +12007,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -12036,7 +12051,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>351</v>
+        <v>299</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -12085,7 +12100,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>407</v>
+        <v>375</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -12112,7 +12127,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>352</v>
+        <v>300</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -12156,7 +12171,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -12205,7 +12220,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12232,7 +12247,7 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12276,7 +12291,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>532</v>
+        <v>301</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12325,7 +12340,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12352,7 +12367,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>531</v>
+        <v>302</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12396,7 +12411,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12445,7 +12460,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12472,7 +12487,7 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12516,7 +12531,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>235</v>
@@ -12565,7 +12580,7 @@
       </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="10"/>
@@ -12592,7 +12607,7 @@
       </c>
       <c r="C164" s="41"/>
       <c r="D164" s="41" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>237</v>
@@ -12636,7 +12651,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>235</v>
@@ -12685,7 +12700,7 @@
       </c>
       <c r="H166" s="10"/>
       <c r="I166" s="10" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="J166" s="10"/>
       <c r="K166" s="10"/>
@@ -12712,7 +12727,7 @@
       </c>
       <c r="C167" s="41"/>
       <c r="D167" s="41" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>237</v>
@@ -12756,7 +12771,7 @@
         <v>1</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>235</v>
@@ -12805,7 +12820,7 @@
       </c>
       <c r="H169" s="10"/>
       <c r="I169" s="10" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="J169" s="10"/>
       <c r="K169" s="10"/>
@@ -12832,7 +12847,7 @@
       </c>
       <c r="C170" s="41"/>
       <c r="D170" s="41" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>237</v>
@@ -12876,7 +12891,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>235</v>
@@ -12925,7 +12940,7 @@
       </c>
       <c r="H172" s="10"/>
       <c r="I172" s="10" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="J172" s="10"/>
       <c r="K172" s="10"/>
@@ -12952,7 +12967,7 @@
       </c>
       <c r="C173" s="41"/>
       <c r="D173" s="41" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="E173" s="41" t="s">
         <v>237</v>
@@ -12996,7 +13011,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>235</v>
@@ -13045,7 +13060,7 @@
       </c>
       <c r="H175" s="10"/>
       <c r="I175" s="10" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="J175" s="10"/>
       <c r="K175" s="10"/>
@@ -13072,7 +13087,7 @@
       </c>
       <c r="C176" s="41"/>
       <c r="D176" s="41" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="E176" s="41" t="s">
         <v>237</v>
@@ -13116,7 +13131,7 @@
         <v>1</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>235</v>
@@ -13165,7 +13180,7 @@
       </c>
       <c r="H178" s="10"/>
       <c r="I178" s="10" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="J178" s="10"/>
       <c r="K178" s="10"/>
@@ -13192,7 +13207,7 @@
       </c>
       <c r="C179" s="41"/>
       <c r="D179" s="41" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="E179" s="41" t="s">
         <v>237</v>
@@ -13231,113 +13246,233 @@
       <c r="W179" s="41"/>
       <c r="X179" s="41"/>
     </row>
-    <row r="180" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A180" s="42" t="b">
+    <row r="180" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A180" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B180" s="42" t="s">
+      <c r="B180" s="40" t="s">
+        <v>540</v>
+      </c>
+      <c r="C180" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D180" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E180" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F180" s="40"/>
+      <c r="G180" s="40"/>
+      <c r="H180" s="40"/>
+      <c r="I180" s="40"/>
+      <c r="J180" s="40"/>
+      <c r="K180" s="40"/>
+      <c r="L180" s="40"/>
+      <c r="M180" s="40"/>
+      <c r="N180" s="40"/>
+      <c r="O180" s="40"/>
+      <c r="P180" s="40"/>
+      <c r="Q180" s="40"/>
+      <c r="R180" s="40"/>
+      <c r="S180" s="40"/>
+      <c r="T180" s="40"/>
+      <c r="U180" s="40"/>
+      <c r="V180" s="40"/>
+      <c r="W180" s="40"/>
+      <c r="X180" s="40"/>
+    </row>
+    <row r="181" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="10"/>
+      <c r="B181" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C181" s="10"/>
+      <c r="D181" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E181" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F181" s="10"/>
+      <c r="G181" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H181" s="10"/>
+      <c r="I181" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="J181" s="10"/>
+      <c r="K181" s="10"/>
+      <c r="L181" s="10"/>
+      <c r="M181" s="10"/>
+      <c r="N181" s="10"/>
+      <c r="O181" s="10"/>
+      <c r="P181" s="10"/>
+      <c r="Q181" s="10"/>
+      <c r="R181" s="10"/>
+      <c r="S181" s="10"/>
+      <c r="T181" s="10"/>
+      <c r="U181" s="10"/>
+      <c r="V181" s="10"/>
+      <c r="W181" s="10"/>
+      <c r="X181" s="10"/>
+      <c r="Y181" s="15"/>
+      <c r="Z181" s="15"/>
+    </row>
+    <row r="182" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A182" s="41"/>
+      <c r="B182" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C182" s="41"/>
+      <c r="D182" s="41" t="s">
+        <v>541</v>
+      </c>
+      <c r="E182" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F182" s="41"/>
+      <c r="G182" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H182" s="41"/>
+      <c r="I182" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J182" s="41"/>
+      <c r="K182" s="41">
+        <v>0</v>
+      </c>
+      <c r="L182" s="41">
+        <v>1</v>
+      </c>
+      <c r="M182" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N182" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O182" s="41"/>
+      <c r="P182" s="41"/>
+      <c r="Q182" s="41"/>
+      <c r="R182" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S182" s="41"/>
+      <c r="T182" s="41"/>
+      <c r="U182" s="41"/>
+      <c r="V182" s="41"/>
+      <c r="W182" s="41"/>
+      <c r="X182" s="41"/>
+    </row>
+    <row r="183" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A183" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B183" s="42" t="s">
         <v>284</v>
       </c>
-      <c r="C180" s="42" t="s">
+      <c r="C183" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="D180" s="42" t="s">
+      <c r="D183" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="E180" s="42" t="s">
+      <c r="E183" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F180" s="42"/>
-      <c r="G180" s="42"/>
-      <c r="H180" s="43"/>
-      <c r="I180" s="43"/>
-      <c r="J180" s="42"/>
-      <c r="K180" s="42"/>
-      <c r="L180" s="42"/>
-      <c r="M180" s="42"/>
-      <c r="N180" s="42"/>
-      <c r="O180" s="42"/>
-      <c r="P180" s="42"/>
-      <c r="Q180" s="42"/>
-      <c r="R180" s="42"/>
-      <c r="S180" s="42"/>
-      <c r="T180" s="42"/>
-      <c r="U180" s="42"/>
-      <c r="V180" s="42"/>
-      <c r="W180" s="42"/>
-      <c r="X180" s="42"/>
-    </row>
-    <row r="181" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A181" s="42" t="b">
+      <c r="F183" s="42"/>
+      <c r="G183" s="42"/>
+      <c r="H183" s="43"/>
+      <c r="I183" s="43"/>
+      <c r="J183" s="42"/>
+      <c r="K183" s="42"/>
+      <c r="L183" s="42"/>
+      <c r="M183" s="42"/>
+      <c r="N183" s="42"/>
+      <c r="O183" s="42"/>
+      <c r="P183" s="42"/>
+      <c r="Q183" s="42"/>
+      <c r="R183" s="42"/>
+      <c r="S183" s="42"/>
+      <c r="T183" s="42"/>
+      <c r="U183" s="42"/>
+      <c r="V183" s="42"/>
+      <c r="W183" s="42"/>
+      <c r="X183" s="42"/>
+    </row>
+    <row r="184" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A184" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B181" s="42" t="s">
-        <v>548</v>
-      </c>
-      <c r="C181" s="42" t="s">
-        <v>549</v>
-      </c>
-      <c r="D181" s="42" t="s">
-        <v>549</v>
-      </c>
-      <c r="E181" s="42" t="s">
+      <c r="B184" s="42" t="s">
+        <v>543</v>
+      </c>
+      <c r="C184" s="42" t="s">
+        <v>544</v>
+      </c>
+      <c r="D184" s="42" t="s">
+        <v>544</v>
+      </c>
+      <c r="E184" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F181" s="42"/>
-      <c r="G181" s="42"/>
-      <c r="H181" s="43"/>
-      <c r="I181" s="43"/>
-      <c r="J181" s="42"/>
-      <c r="K181" s="42"/>
-      <c r="L181" s="42"/>
-      <c r="M181" s="42"/>
-      <c r="N181" s="42"/>
-      <c r="O181" s="42"/>
-      <c r="P181" s="42"/>
-      <c r="Q181" s="42"/>
-      <c r="R181" s="42"/>
-      <c r="S181" s="42"/>
-      <c r="T181" s="42"/>
-      <c r="U181" s="42"/>
-      <c r="V181" s="42"/>
-      <c r="W181" s="42"/>
-      <c r="X181" s="42"/>
-    </row>
-    <row r="182" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="42" t="b">
+      <c r="F184" s="42"/>
+      <c r="G184" s="42"/>
+      <c r="H184" s="43"/>
+      <c r="I184" s="43"/>
+      <c r="J184" s="42"/>
+      <c r="K184" s="42"/>
+      <c r="L184" s="42"/>
+      <c r="M184" s="42"/>
+      <c r="N184" s="42"/>
+      <c r="O184" s="42"/>
+      <c r="P184" s="42"/>
+      <c r="Q184" s="42"/>
+      <c r="R184" s="42"/>
+      <c r="S184" s="42"/>
+      <c r="T184" s="42"/>
+      <c r="U184" s="42"/>
+      <c r="V184" s="42"/>
+      <c r="W184" s="42"/>
+      <c r="X184" s="42"/>
+    </row>
+    <row r="185" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B182" s="42" t="s">
+      <c r="B185" s="42" t="s">
         <v>355</v>
       </c>
-      <c r="C182" s="42" t="s">
+      <c r="C185" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="D182" s="42" t="s">
+      <c r="D185" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="E182" s="42" t="s">
+      <c r="E185" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F182" s="42"/>
-      <c r="G182" s="42"/>
-      <c r="H182" s="43"/>
-      <c r="I182" s="43"/>
-      <c r="J182" s="42"/>
-      <c r="K182" s="42"/>
-      <c r="L182" s="42"/>
-      <c r="M182" s="42"/>
-      <c r="N182" s="42"/>
-      <c r="O182" s="42"/>
-      <c r="P182" s="42"/>
-      <c r="Q182" s="42"/>
-      <c r="R182" s="42"/>
-      <c r="S182" s="42"/>
-      <c r="T182" s="42"/>
-      <c r="U182" s="42"/>
-      <c r="V182" s="42"/>
-      <c r="W182" s="42"/>
-      <c r="X182" s="42"/>
+      <c r="F185" s="42"/>
+      <c r="G185" s="42"/>
+      <c r="H185" s="43"/>
+      <c r="I185" s="43"/>
+      <c r="J185" s="42"/>
+      <c r="K185" s="42"/>
+      <c r="L185" s="42"/>
+      <c r="M185" s="42"/>
+      <c r="N185" s="42"/>
+      <c r="O185" s="42"/>
+      <c r="P185" s="42"/>
+      <c r="Q185" s="42"/>
+      <c r="R185" s="42"/>
+      <c r="S185" s="42"/>
+      <c r="T185" s="42"/>
+      <c r="U185" s="42"/>
+      <c r="V185" s="42"/>
+      <c r="W185" s="42"/>
+      <c r="X185" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -13356,11 +13491,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13474,1298 +13609,1298 @@
       </c>
       <c r="M3" s="32"/>
     </row>
-    <row r="4" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" s="49" t="s">
         <v>305</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50" t="s">
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49" t="s">
+        <v>432</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G4" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+    </row>
+    <row r="5" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A5" s="49" t="s">
+        <v>306</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49" t="s">
+        <v>462</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G5" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+    </row>
+    <row r="6" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49" t="s">
+        <v>483</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G6" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+    </row>
+    <row r="7" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A7" s="49" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49" t="s">
+        <v>447</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G7" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+    </row>
+    <row r="8" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A8" s="49" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49" t="s">
+        <v>482</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G8" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+    </row>
+    <row r="9" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" s="49" t="s">
+        <v>488</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49" t="s">
+        <v>442</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G9" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+    </row>
+    <row r="10" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="49" t="s">
+        <v>489</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49" t="s">
+        <v>444</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G10" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+    </row>
+    <row r="11" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="49" t="s">
+        <v>490</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49" t="s">
+        <v>445</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G11" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+    </row>
+    <row r="12" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="49" t="s">
+        <v>491</v>
+      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49" t="s">
+        <v>443</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G12" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+    </row>
+    <row r="13" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" s="49" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49" t="s">
+        <v>446</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G13" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+    </row>
+    <row r="14" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="49" t="s">
+        <v>311</v>
+      </c>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49" t="s">
+        <v>472</v>
+      </c>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G14" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+    </row>
+    <row r="15" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A15" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49" t="s">
+        <v>439</v>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G15" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+    </row>
+    <row r="16" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="49" t="s">
+        <v>337</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49" t="s">
+        <v>473</v>
+      </c>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G16" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+    </row>
+    <row r="17" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G17" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49" t="s">
+        <v>341</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>486</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G18" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A19" s="49" t="s">
+        <v>331</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49" t="s">
+        <v>471</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G19" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+    </row>
+    <row r="20" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A20" s="49" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49" t="s">
+        <v>458</v>
+      </c>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G20" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+    </row>
+    <row r="21" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="49" t="s">
+        <v>492</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49" t="s">
+        <v>460</v>
+      </c>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G21" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+    </row>
+    <row r="22" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="49" t="s">
+        <v>493</v>
+      </c>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49" t="s">
+        <v>456</v>
+      </c>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G22" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+    </row>
+    <row r="23" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="49" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49" t="s">
+        <v>457</v>
+      </c>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G23" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+    </row>
+    <row r="24" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>494</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>453</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G24" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
+        <v>314</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>459</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G25" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>315</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>454</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G26" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="49" t="s">
+        <v>495</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>455</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G27" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
+        <v>340</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>481</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G28" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="49" t="s">
+        <v>484</v>
+      </c>
+      <c r="F29" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G29" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="49" t="s">
+        <v>317</v>
+      </c>
+      <c r="D30" s="49" t="s">
+        <v>440</v>
+      </c>
+      <c r="F30" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G30" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>476</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G31" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="49" t="s">
+        <v>319</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>441</v>
+      </c>
+      <c r="F32" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G32" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="49" t="s">
+        <v>496</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>479</v>
+      </c>
+      <c r="F33" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G33" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="49" t="s">
+        <v>497</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>478</v>
+      </c>
+      <c r="F34" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G34" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="49" t="s">
+        <v>498</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>480</v>
+      </c>
+      <c r="F35" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G35" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="49" t="s">
+        <v>499</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>477</v>
+      </c>
+      <c r="F36" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G36" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="49" t="s">
+        <v>321</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>438</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G37" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="49" t="s">
+        <v>346</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>487</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G38" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>485</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G39" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="D40" s="49" t="s">
+        <v>448</v>
+      </c>
+      <c r="F40" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G40" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="49" t="s">
+        <v>364</v>
+      </c>
+      <c r="D41" s="49" t="s">
+        <v>452</v>
+      </c>
+      <c r="F41" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G41" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="49" t="s">
+        <v>365</v>
+      </c>
+      <c r="D42" s="49" t="s">
+        <v>449</v>
+      </c>
+      <c r="F42" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G42" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="49" t="s">
+        <v>367</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>451</v>
+      </c>
+      <c r="F43" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G43" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="49" t="s">
+        <v>366</v>
+      </c>
+      <c r="D44" s="49" t="s">
+        <v>450</v>
+      </c>
+      <c r="F44" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G44" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="49" t="s">
+        <v>587</v>
+      </c>
+      <c r="D45" s="49" t="s">
+        <v>588</v>
+      </c>
+      <c r="F45" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G45" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="49" t="s">
+        <v>589</v>
+      </c>
+      <c r="D46" s="49" t="s">
+        <v>590</v>
+      </c>
+      <c r="F46" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G46" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="D47" s="49" t="s">
+        <v>475</v>
+      </c>
+      <c r="F47" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G47" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="D48" s="49" t="s">
+        <v>435</v>
+      </c>
+      <c r="F48" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G48" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="49" t="s">
+        <v>325</v>
+      </c>
+      <c r="D49" s="49" t="s">
         <v>436</v>
       </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50" t="s">
+      <c r="F49" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G4" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-    </row>
-    <row r="5" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50" t="s">
+      <c r="G49" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="49" t="s">
+        <v>326</v>
+      </c>
+      <c r="D50" s="49" t="s">
+        <v>434</v>
+      </c>
+      <c r="F50" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G50" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" s="49" t="s">
+        <v>433</v>
+      </c>
+      <c r="F51" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G51" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="D52" s="49" t="s">
+        <v>461</v>
+      </c>
+      <c r="F52" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G52" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="49" t="s">
+        <v>328</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>474</v>
+      </c>
+      <c r="F53" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G53" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="49" t="s">
+        <v>500</v>
+      </c>
+      <c r="D54" s="49" t="s">
+        <v>463</v>
+      </c>
+      <c r="F54" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G54" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="49" t="s">
+        <v>501</v>
+      </c>
+      <c r="D55" s="49" t="s">
+        <v>464</v>
+      </c>
+      <c r="F55" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G55" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="49" t="s">
+        <v>502</v>
+      </c>
+      <c r="D56" s="49" t="s">
+        <v>465</v>
+      </c>
+      <c r="F56" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G56" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="D57" s="49" t="s">
+        <v>466</v>
+      </c>
+      <c r="F57" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="G57" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="49" t="s">
+        <v>504</v>
+      </c>
+      <c r="D58" s="49" t="s">
         <v>467</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50" t="s">
+      <c r="F58" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G5" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-    </row>
-    <row r="6" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
-        <v>307</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50" t="s">
-        <v>488</v>
-      </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50" t="s">
+      <c r="G58" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="49" t="s">
+        <v>505</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>468</v>
+      </c>
+      <c r="F59" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G6" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-    </row>
-    <row r="7" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
-        <v>308</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50" t="s">
-        <v>451</v>
-      </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50" t="s">
+      <c r="G59" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="D60" s="49" t="s">
+        <v>469</v>
+      </c>
+      <c r="F60" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G7" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-    </row>
-    <row r="8" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
-        <v>309</v>
-      </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50" t="s">
-        <v>487</v>
-      </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50" t="s">
+      <c r="G60" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="49" t="s">
+        <v>507</v>
+      </c>
+      <c r="D61" s="49" t="s">
+        <v>470</v>
+      </c>
+      <c r="F61" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G8" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-    </row>
-    <row r="9" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
-        <v>493</v>
-      </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50" t="s">
-        <v>446</v>
-      </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G9" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-    </row>
-    <row r="10" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
-        <v>494</v>
-      </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50" t="s">
-        <v>448</v>
-      </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G10" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-    </row>
-    <row r="11" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="50" t="s">
-        <v>495</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50" t="s">
-        <v>449</v>
-      </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G11" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-    </row>
-    <row r="12" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
-        <v>496</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50" t="s">
-        <v>447</v>
-      </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G12" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-    </row>
-    <row r="13" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
-        <v>310</v>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50" t="s">
-        <v>450</v>
-      </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G13" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-    </row>
-    <row r="14" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="50" t="s">
-        <v>311</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50" t="s">
-        <v>477</v>
-      </c>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G14" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-    </row>
-    <row r="15" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="50" t="s">
-        <v>334</v>
-      </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50" t="s">
-        <v>443</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G15" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-    </row>
-    <row r="16" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
-        <v>337</v>
-      </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50" t="s">
-        <v>478</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G16" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-    </row>
-    <row r="17" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
-        <v>320</v>
-      </c>
-      <c r="D17" s="50" t="s">
-        <v>441</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G17" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
-        <v>341</v>
-      </c>
-      <c r="D18" s="50" t="s">
-        <v>491</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G18" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="50" t="s">
-        <v>331</v>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50" t="s">
-        <v>476</v>
-      </c>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G19" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-    </row>
-    <row r="20" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
-        <v>312</v>
-      </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50" t="s">
-        <v>463</v>
-      </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G20" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-    </row>
-    <row r="21" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
-        <v>497</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50" t="s">
-        <v>465</v>
-      </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G21" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-    </row>
-    <row r="22" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
-        <v>498</v>
-      </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50" t="s">
-        <v>461</v>
-      </c>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G22" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-    </row>
-    <row r="23" spans="1:13" s="51" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="50" t="s">
-        <v>313</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50" t="s">
-        <v>462</v>
-      </c>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G23" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-    </row>
-    <row r="24" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="50" t="s">
-        <v>499</v>
-      </c>
-      <c r="D24" s="50" t="s">
-        <v>458</v>
-      </c>
-      <c r="F24" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G24" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
-        <v>314</v>
-      </c>
-      <c r="D25" s="50" t="s">
-        <v>464</v>
-      </c>
-      <c r="F25" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G25" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="50" t="s">
-        <v>315</v>
-      </c>
-      <c r="D26" s="50" t="s">
-        <v>459</v>
-      </c>
-      <c r="F26" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G26" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
-        <v>500</v>
-      </c>
-      <c r="D27" s="50" t="s">
-        <v>460</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G27" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
-        <v>340</v>
-      </c>
-      <c r="D28" s="50" t="s">
-        <v>486</v>
-      </c>
-      <c r="F28" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G28" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
-        <v>316</v>
-      </c>
-      <c r="D29" s="50" t="s">
-        <v>489</v>
-      </c>
-      <c r="F29" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G29" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50" t="s">
-        <v>317</v>
-      </c>
-      <c r="D30" s="50" t="s">
-        <v>444</v>
-      </c>
-      <c r="F30" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G30" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
-        <v>318</v>
-      </c>
-      <c r="D31" s="50" t="s">
-        <v>481</v>
-      </c>
-      <c r="F31" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G31" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50" t="s">
-        <v>319</v>
-      </c>
-      <c r="D32" s="50" t="s">
-        <v>445</v>
-      </c>
-      <c r="F32" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G32" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
-        <v>501</v>
-      </c>
-      <c r="D33" s="50" t="s">
-        <v>484</v>
-      </c>
-      <c r="F33" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G33" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50" t="s">
-        <v>502</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>483</v>
-      </c>
-      <c r="F34" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G34" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="50" t="s">
-        <v>503</v>
-      </c>
-      <c r="D35" s="50" t="s">
-        <v>485</v>
-      </c>
-      <c r="F35" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G35" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="50" t="s">
-        <v>504</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>482</v>
-      </c>
-      <c r="F36" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G36" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
-        <v>321</v>
-      </c>
-      <c r="D37" s="50" t="s">
-        <v>442</v>
-      </c>
-      <c r="F37" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G37" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I37" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
-        <v>346</v>
-      </c>
-      <c r="D38" s="50" t="s">
-        <v>492</v>
-      </c>
-      <c r="F38" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G38" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H38" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="50" t="s">
-        <v>322</v>
-      </c>
-      <c r="D39" s="50" t="s">
-        <v>490</v>
-      </c>
-      <c r="F39" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G39" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
-        <v>375</v>
-      </c>
-      <c r="D40" s="50" t="s">
-        <v>452</v>
-      </c>
-      <c r="F40" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G40" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
-        <v>374</v>
-      </c>
-      <c r="D41" s="50" t="s">
-        <v>453</v>
-      </c>
-      <c r="F41" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G41" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H41" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I41" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
-        <v>364</v>
-      </c>
-      <c r="D42" s="50" t="s">
-        <v>457</v>
-      </c>
-      <c r="F42" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G42" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="50" t="s">
-        <v>365</v>
-      </c>
-      <c r="D43" s="50" t="s">
-        <v>454</v>
-      </c>
-      <c r="F43" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G43" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H43" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
-        <v>367</v>
-      </c>
-      <c r="D44" s="50" t="s">
-        <v>456</v>
-      </c>
-      <c r="F44" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G44" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I44" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="50" t="s">
-        <v>366</v>
-      </c>
-      <c r="D45" s="50" t="s">
-        <v>455</v>
-      </c>
-      <c r="F45" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G45" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H45" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="50" t="s">
-        <v>323</v>
-      </c>
-      <c r="D46" s="50" t="s">
-        <v>480</v>
-      </c>
-      <c r="F46" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G46" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H46" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I46" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="50" t="s">
-        <v>324</v>
-      </c>
-      <c r="D47" s="50" t="s">
-        <v>439</v>
-      </c>
-      <c r="F47" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G47" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H47" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="50" t="s">
-        <v>325</v>
-      </c>
-      <c r="D48" s="50" t="s">
-        <v>440</v>
-      </c>
-      <c r="F48" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G48" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
-        <v>326</v>
-      </c>
-      <c r="D49" s="50" t="s">
-        <v>438</v>
-      </c>
-      <c r="F49" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G49" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="50" t="s">
-        <v>327</v>
-      </c>
-      <c r="D50" s="50" t="s">
-        <v>437</v>
-      </c>
-      <c r="F50" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G50" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="50" t="s">
-        <v>353</v>
-      </c>
-      <c r="D51" s="50" t="s">
-        <v>466</v>
-      </c>
-      <c r="F51" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G51" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="D52" s="50" t="s">
-        <v>479</v>
-      </c>
-      <c r="F52" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G52" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H52" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I52" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="50" t="s">
-        <v>505</v>
-      </c>
-      <c r="D53" s="50" t="s">
-        <v>468</v>
-      </c>
-      <c r="F53" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G53" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H53" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="50" t="s">
-        <v>506</v>
-      </c>
-      <c r="D54" s="50" t="s">
-        <v>469</v>
-      </c>
-      <c r="F54" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G54" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I54" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="50" t="s">
-        <v>507</v>
-      </c>
-      <c r="D55" s="50" t="s">
-        <v>470</v>
-      </c>
-      <c r="F55" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G55" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="50" t="s">
-        <v>508</v>
-      </c>
-      <c r="D56" s="50" t="s">
-        <v>471</v>
-      </c>
-      <c r="F56" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G56" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H56" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I56" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="50" t="s">
-        <v>509</v>
-      </c>
-      <c r="D57" s="50" t="s">
-        <v>472</v>
-      </c>
-      <c r="F57" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G57" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="50" t="s">
-        <v>510</v>
-      </c>
-      <c r="D58" s="50" t="s">
-        <v>473</v>
-      </c>
-      <c r="F58" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G58" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H58" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I58" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="50" t="s">
-        <v>511</v>
-      </c>
-      <c r="D59" s="50" t="s">
-        <v>474</v>
-      </c>
-      <c r="F59" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G59" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H59" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="50" t="s">
-        <v>512</v>
-      </c>
-      <c r="D60" s="50" t="s">
-        <v>475</v>
-      </c>
-      <c r="F60" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="G60" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H60" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49" t="s">
-        <v>550</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>573</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="G61" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H61" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I61" s="14" t="b">
+      <c r="G61" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" s="49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
-        <v>551</v>
+      <c r="A62" s="48" t="s">
+        <v>545</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="F62" s="14" t="s">
         <v>286</v>
@@ -14781,11 +14916,11 @@
       </c>
     </row>
     <row r="63" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49" t="s">
-        <v>552</v>
+      <c r="A63" s="48" t="s">
+        <v>546</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="F63" s="14" t="s">
         <v>286</v>
@@ -14801,11 +14936,11 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49" t="s">
-        <v>553</v>
+      <c r="A64" s="48" t="s">
+        <v>547</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F64" s="14" t="s">
         <v>286</v>
@@ -14821,11 +14956,11 @@
       </c>
     </row>
     <row r="65" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="49" t="s">
-        <v>554</v>
+      <c r="A65" s="48" t="s">
+        <v>548</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>286</v>
@@ -14841,11 +14976,11 @@
       </c>
     </row>
     <row r="66" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
-        <v>555</v>
+      <c r="A66" s="48" t="s">
+        <v>549</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>286</v>
@@ -14861,11 +14996,11 @@
       </c>
     </row>
     <row r="67" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="49" t="s">
-        <v>556</v>
+      <c r="A67" s="48" t="s">
+        <v>550</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="F67" s="14" t="s">
         <v>286</v>
@@ -14881,11 +15016,11 @@
       </c>
     </row>
     <row r="68" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
-        <v>557</v>
+      <c r="A68" s="48" t="s">
+        <v>551</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="F68" s="14" t="s">
         <v>286</v>
@@ -14901,11 +15036,11 @@
       </c>
     </row>
     <row r="69" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="49" t="s">
-        <v>558</v>
+      <c r="A69" s="48" t="s">
+        <v>552</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>286</v>
@@ -14921,11 +15056,11 @@
       </c>
     </row>
     <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
-        <v>559</v>
+      <c r="A70" s="48" t="s">
+        <v>553</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="F70" s="14" t="s">
         <v>286</v>
@@ -14941,11 +15076,11 @@
       </c>
     </row>
     <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
-        <v>560</v>
+      <c r="A71" s="48" t="s">
+        <v>554</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>286</v>
@@ -14961,11 +15096,11 @@
       </c>
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
-        <v>561</v>
+      <c r="A72" s="48" t="s">
+        <v>555</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>286</v>
@@ -14981,11 +15116,11 @@
       </c>
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
-        <v>562</v>
+      <c r="A73" s="48" t="s">
+        <v>556</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>286</v>
@@ -15002,10 +15137,10 @@
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>286</v>
@@ -15022,10 +15157,10 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>286</v>
@@ -15042,10 +15177,10 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>286</v>
@@ -15062,10 +15197,10 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>286</v>
@@ -15082,10 +15217,10 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>286</v>
@@ -15097,6 +15232,26 @@
         <v>0</v>
       </c>
       <c r="I78" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="F79" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G79" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" s="14" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest RBSA queried distribution files. Some code refactoring. Closes #7.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -5398,7 +5398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5525,7 +5527,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="23" t="s">
@@ -5533,7 +5535,7 @@
       </c>
       <c r="E9" s="23" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$1.68/hour</v>
+        <v>$6.72/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>202</v>
@@ -5688,14 +5690,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="22"/>
     </row>

</xml_diff>

<commit_message>
Latest measures and RBSA-based PNW probability distributions.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -5398,9 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Latest measures. Updated sample results.
</commit_message>
<xml_diff>
--- a/projects/res_stock_pnw_existing.xlsx
+++ b/projects/res_stock_pnw_existing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="8295" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="8295" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -5323,9 +5323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5615,14 +5613,14 @@
       </c>
       <c r="B24" s="17">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)-1)))</f>
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$30,0)))=0,"",INDEX(Lookups!$C$19:$AI$28,2,3*MATCH(Setup!$B20,Lookups!$A$19:$A$29,0)))</f>
         <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D24" s="26">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="22"/>
     </row>
@@ -5962,7 +5960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>